<commit_message>
Improve labels in reweighted CC spreadsheet
</commit_message>
<xml_diff>
--- a/Config/Reweighted_GlobocanCC_rates.xlsx
+++ b/Config/Reweighted_GlobocanCC_rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0387EA61-FB68-4ADD-A93F-16B83C2059C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B97C17D-52E4-4A8A-B447-72D9D9AF53A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,41 +26,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>HIV+ RR</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimated </t>
-  </si>
-  <si>
     <t xml:space="preserve">Check estimates </t>
   </si>
   <si>
     <t xml:space="preserve">Age </t>
   </si>
   <si>
-    <t>Cases</t>
-  </si>
-  <si>
-    <t>Pop</t>
-  </si>
-  <si>
-    <t>HIV+pop</t>
-  </si>
-  <si>
-    <t>HIV-pop</t>
-  </si>
-  <si>
-    <t>RR HIV+ vs HIV-</t>
-  </si>
-  <si>
-    <t>HIV+</t>
-  </si>
-  <si>
-    <t>HIV-</t>
-  </si>
-  <si>
     <t>CCcasesHIV+</t>
   </si>
   <si>
@@ -109,67 +85,106 @@
     <t>Total</t>
   </si>
   <si>
-    <t>HIV+ 4x higher risk for cervical cancer</t>
-  </si>
-  <si>
-    <t>KZN CC rate (HIV 4x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Observed Globocan 2018 </t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>SADHS 2016</t>
-  </si>
-  <si>
-    <t>CCrateSA</t>
-  </si>
-  <si>
-    <t>HIVSA all Females</t>
-  </si>
-  <si>
-    <t>CCrateHIV+</t>
-  </si>
-  <si>
-    <t>CCrateHIV-</t>
-  </si>
-  <si>
     <t>CCtotal</t>
   </si>
   <si>
     <t>Weighted CCrateSA</t>
   </si>
   <si>
-    <t>SSA Pop 2016</t>
-  </si>
-  <si>
-    <t>Mults</t>
-  </si>
-  <si>
-    <t>Mults Adjusted</t>
-  </si>
-  <si>
-    <t>Mults for broad age groups</t>
-  </si>
-  <si>
     <t>KZN CC rate (HIV 4x risk) - adjusted older ages</t>
   </si>
   <si>
-    <t>AHRI KZN 2016</t>
-  </si>
-  <si>
-    <t>HIV KZN</t>
-  </si>
-  <si>
     <t>Pop KZN</t>
   </si>
   <si>
-    <t>Estimated</t>
-  </si>
-  <si>
     <t>Age Group</t>
+  </si>
+  <si>
+    <t>Observed DHS 2016 HIV Prevalence in SA</t>
+  </si>
+  <si>
+    <t>Observed Globocan 2018 CC incidence in SA</t>
+  </si>
+  <si>
+    <t>CC rate HIV+</t>
+  </si>
+  <si>
+    <t>CC rate HIV-</t>
+  </si>
+  <si>
+    <t>25-34</t>
+  </si>
+  <si>
+    <t>35-44</t>
+  </si>
+  <si>
+    <t>45-54</t>
+  </si>
+  <si>
+    <t>55-64</t>
+  </si>
+  <si>
+    <t>65+</t>
+  </si>
+  <si>
+    <t>Observed AHRI 2016 HIV prevalence in KZN</t>
+  </si>
+  <si>
+    <t>HIV SA (all females)</t>
+  </si>
+  <si>
+    <t>HIV KZN (all females)</t>
+  </si>
+  <si>
+    <t>set equal to 45-49 age group</t>
+  </si>
+  <si>
+    <t>Statistics SA 2016 Population in KZN</t>
+  </si>
+  <si>
+    <t>Cases SA</t>
+  </si>
+  <si>
+    <t>Pop SA</t>
+  </si>
+  <si>
+    <t>CC rate SA</t>
+  </si>
+  <si>
+    <t>HIV+ Pop</t>
+  </si>
+  <si>
+    <t>HIV- Pop</t>
+  </si>
+  <si>
+    <t>Calculated population in KZN by HIV status</t>
+  </si>
+  <si>
+    <t>Estimated CC incidence rates in SA by HIV status</t>
+  </si>
+  <si>
+    <t>Estimated CC cases by HIV status and CC incidence rate in KZN</t>
+  </si>
+  <si>
+    <t>CC cases HIV+</t>
+  </si>
+  <si>
+    <t>CC cases HIV-</t>
+  </si>
+  <si>
+    <t>CC rate KZN</t>
+  </si>
+  <si>
+    <t>Multiplier on Globocan 2018 data</t>
+  </si>
+  <si>
+    <t>Adjusted multipliers</t>
+  </si>
+  <si>
+    <t>Multipliers for broad age groups</t>
   </si>
 </sst>
 </file>
@@ -307,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -384,11 +399,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -424,9 +461,7 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -455,15 +490,31 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,7 +621,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Observed Globocan 2018 </c:v>
+                  <c:v>Observed Globocan 2018 CC incidence in SA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -700,7 +751,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'CC rates'!$AC$3</c:f>
+              <c:f>'CC rates'!$AB$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -779,7 +830,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CC rates'!$AC$4:$AC$15</c:f>
+              <c:f>'CC rates'!$AB$4:$AB$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1732,13 +1783,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -1967,55 +2018,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF959"/>
+  <dimension ref="A1:AE959"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="7.625" customWidth="1"/>
-    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="7.625" customWidth="1"/>
-    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.625" customWidth="1"/>
-    <col min="12" max="16" width="7.625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="7.625" customWidth="1"/>
-    <col min="21" max="21" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.625" customWidth="1"/>
-    <col min="25" max="25" width="7.625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.625" style="20" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5" customWidth="1"/>
-    <col min="29" max="29" width="23.375" customWidth="1"/>
-    <col min="30" max="31" width="7.625" customWidth="1"/>
-    <col min="32" max="32" width="13.625" customWidth="1"/>
+    <col min="1" max="3" width="7.625" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.625" customWidth="1"/>
+    <col min="7" max="7" width="1.625" style="49" customWidth="1"/>
+    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.375" customWidth="1"/>
+    <col min="11" max="14" width="7.625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10.125" customWidth="1"/>
+    <col min="16" max="16" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.375" customWidth="1"/>
+    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="19" max="19" width="10.875" customWidth="1"/>
+    <col min="20" max="20" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.75" customWidth="1"/>
+    <col min="22" max="22" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.625" customWidth="1"/>
+    <col min="24" max="24" width="7.625" style="20" customWidth="1"/>
+    <col min="25" max="25" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.625" style="20" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.375" customWidth="1"/>
+    <col min="29" max="30" width="7.625" customWidth="1"/>
+    <col min="31" max="31" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+    <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="52"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="38" t="s">
+      <c r="H1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="38">
+      <c r="I1" s="36">
         <v>4</v>
       </c>
+      <c r="J1" s="25"/>
       <c r="K1" s="25"/>
       <c r="L1" s="25"/>
       <c r="M1" s="25"/>
@@ -2032,1480 +2084,1368 @@
       <c r="X1" s="25"/>
       <c r="Y1" s="25"/>
       <c r="Z1" s="25"/>
-      <c r="AA1" s="25"/>
-      <c r="AB1" s="26"/>
-    </row>
-    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="33" t="s">
-        <v>31</v>
+      <c r="AA1" s="26"/>
+    </row>
+    <row r="2" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="54" t="s">
+        <v>25</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="31" t="s">
+      <c r="H2" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="56"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="24" t="s">
-        <v>2</v>
-      </c>
+      <c r="L2" s="25"/>
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="31" t="s">
+      <c r="P2" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="56"/>
+      <c r="T2" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="26"/>
+    </row>
+    <row r="3" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="25"/>
+      <c r="K3" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="27"/>
+      <c r="P3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="26"/>
-    </row>
-    <row r="3" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="S3" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="T3" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="V3" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="W3" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="44" t="s">
+      <c r="T3" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="Z3" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA3" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB3" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC3" s="46" t="s">
-        <v>42</v>
-      </c>
+      <c r="U3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="W3" s="25"/>
+      <c r="X3" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z3" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA3" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB3" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
       <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
-    </row>
-    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="35">
+    </row>
+    <row r="4" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="33">
         <v>100</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="34">
         <f>B4/(D4/100000)</f>
         <v>2559474</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="35">
         <v>3.9070527772503256</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="32">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="F4" s="27">
-        <f t="shared" ref="F4:F16" si="0">E4*C4</f>
-        <v>151008.96599999999</v>
-      </c>
-      <c r="G4" s="27">
-        <v>2364630.3199999998</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="39">
-        <f t="shared" ref="I4:I16" si="1">J$1*J4</f>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="37">
+        <f t="shared" ref="H4:H16" si="0">I$1*I4</f>
         <v>13.278004340697793</v>
       </c>
-      <c r="J4" s="39">
-        <f t="shared" ref="J4:J16" si="2">D4/(J$1*E4+(1-E4))</f>
+      <c r="I4" s="37">
+        <f>D4/(I$1*E4+(1-E4))</f>
         <v>3.3195010851744482</v>
       </c>
-      <c r="K4" s="25"/>
-      <c r="L4" s="26">
-        <f t="shared" ref="L4:M4" si="3">I4*F4/100000</f>
-        <v>20.050977060322854</v>
-      </c>
-      <c r="M4" s="26">
-        <f t="shared" si="3"/>
-        <v>78.493929132764023</v>
-      </c>
-      <c r="N4" s="26">
-        <f t="shared" ref="N4:N16" si="4">SUM(L4+M4)</f>
-        <v>98.544906193086874</v>
-      </c>
-      <c r="O4" s="28">
-        <f t="shared" ref="O4:O16" si="5">(I4*(F4/C4))+(J4*(G4/C4))</f>
-        <v>3.850201494255729</v>
-      </c>
-      <c r="P4" s="28">
-        <f t="shared" ref="P4:P16" si="6">I4/J4</f>
-        <v>4</v>
-      </c>
-      <c r="Q4" s="41">
+      <c r="J4" s="25"/>
+      <c r="K4" s="26" t="e">
+        <f>H4*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L4" s="26" t="e">
+        <f>I4*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M4" s="26" t="e">
+        <f t="shared" ref="M4:M16" si="1">SUM(K4+L4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N4" s="28" t="e">
+        <f>(H4*(#REF!/C4))+(I4*(#REF!/C4))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O4" s="28"/>
+      <c r="P4" s="39">
         <f>0.0935</f>
         <v>9.35E-2</v>
       </c>
-      <c r="R4" s="42">
+      <c r="Q4" s="40">
         <v>538265</v>
       </c>
-      <c r="S4" s="40">
-        <f t="shared" ref="S4:S16" si="7">Q4*R4</f>
+      <c r="R4" s="38">
+        <f t="shared" ref="R4:R16" si="2">P4*Q4</f>
         <v>50327.777499999997</v>
       </c>
-      <c r="T4" s="40">
-        <f t="shared" ref="T4:T16" si="8">R4-S4</f>
+      <c r="S4" s="38">
+        <f t="shared" ref="S4:S16" si="3">Q4-R4</f>
         <v>487937.22250000003</v>
       </c>
-      <c r="U4" s="43">
-        <f t="shared" ref="U4:U16" si="9">I4*S4/100000</f>
+      <c r="T4" s="41">
+        <f t="shared" ref="T4:T16" si="4">H4*R4/100000</f>
         <v>6.6825244810267268</v>
       </c>
-      <c r="V4" s="43">
-        <f t="shared" ref="V4:V16" si="10">J4*T4/100000</f>
+      <c r="U4" s="41">
+        <f t="shared" ref="U4:U16" si="5">I4*S4/100000</f>
         <v>16.197081395857563</v>
       </c>
-      <c r="W4" s="43">
-        <f t="shared" ref="W4:W16" si="11">(U4+V4)/R4*100000</f>
+      <c r="V4" s="41">
+        <f t="shared" ref="V4:V16" si="6">(T4+U4)/Q4*100000</f>
         <v>4.2506211395658813</v>
       </c>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="51">
+      <c r="W4" s="25"/>
+      <c r="X4" s="48">
         <v>4</v>
       </c>
-      <c r="Z4" s="34">
-        <f t="shared" ref="Z4:Z16" si="12">W4/D4</f>
+      <c r="Y4" s="32">
+        <f>V4/D4</f>
         <v>1.0879354290569245</v>
       </c>
-      <c r="AA4" s="34">
-        <f>Z4</f>
+      <c r="Z4" s="32">
+        <f>Y4</f>
         <v>1.0879354290569245</v>
       </c>
-      <c r="AB4" s="47">
-        <f>AVERAGE(Z4:Z6)</f>
+      <c r="AA4" s="45">
+        <f>AVERAGE(Y4:Y6)</f>
         <v>1.2195984455181634</v>
       </c>
-      <c r="AC4" s="48">
-        <f t="shared" ref="AC4:AC15" si="13">D4*AA4</f>
+      <c r="AB4" s="46">
+        <f>D4*Z4</f>
         <v>4.2506211395658813</v>
       </c>
+      <c r="AC4" s="15"/>
       <c r="AD4" s="15"/>
       <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-    </row>
-    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="35">
+    </row>
+    <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="33">
         <v>503</v>
       </c>
-      <c r="C5" s="36">
-        <f t="shared" ref="C5:C15" si="14">B5/(D5/100000)</f>
+      <c r="C5" s="34">
+        <f t="shared" ref="C5:C15" si="7">B5/(D5/100000)</f>
         <v>2550891.9999999995</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="35">
         <v>19.718592555074853</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="32">
         <v>0.16700000000000001</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="37">
         <f t="shared" si="0"/>
-        <v>425998.96399999992</v>
-      </c>
-      <c r="G5" s="27">
-        <v>2213594.0960000004</v>
-      </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="39">
+        <v>52.547881559160174</v>
+      </c>
+      <c r="I5" s="37">
+        <f>D5/(I$1*E5+(1-E5))</f>
+        <v>13.136970389790044</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26" t="e">
+        <f>H5*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L5" s="26" t="e">
+        <f>I5*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M5" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>52.547881559160174</v>
-      </c>
-      <c r="J5" s="39">
-        <f t="shared" si="2"/>
-        <v>13.136970389790044</v>
-      </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="26">
-        <f t="shared" ref="L5:M5" si="15">I5*F5/100000</f>
-        <v>223.85343104596936</v>
-      </c>
-      <c r="M5" s="26">
-        <f t="shared" si="15"/>
-        <v>290.79920094166062</v>
-      </c>
-      <c r="N5" s="26">
-        <f t="shared" si="4"/>
-        <v>514.65263198763</v>
-      </c>
-      <c r="O5" s="28">
-        <f t="shared" si="5"/>
-        <v>20.175398722785211</v>
-      </c>
-      <c r="P5" s="28">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q5" s="41">
+        <v>#REF!</v>
+      </c>
+      <c r="N5" s="28" t="e">
+        <f>(H5*(#REF!/C5))+(I5*(#REF!/C5))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O5" s="28"/>
+      <c r="P5" s="39">
         <f>0.3342</f>
         <v>0.3342</v>
       </c>
-      <c r="R5" s="42">
+      <c r="Q5" s="40">
         <v>543645</v>
       </c>
-      <c r="S5" s="40">
-        <f t="shared" si="7"/>
+      <c r="R5" s="38">
+        <f t="shared" si="2"/>
         <v>181686.15899999999</v>
       </c>
-      <c r="T5" s="40">
-        <f t="shared" si="8"/>
+      <c r="S5" s="38">
+        <f t="shared" si="3"/>
         <v>361958.84100000001</v>
       </c>
-      <c r="U5" s="43">
-        <f t="shared" si="9"/>
+      <c r="T5" s="41">
+        <f t="shared" si="4"/>
         <v>95.472227640707416</v>
       </c>
-      <c r="V5" s="43">
-        <f t="shared" si="10"/>
+      <c r="U5" s="41">
+        <f t="shared" si="5"/>
         <v>47.550425765397222</v>
       </c>
-      <c r="W5" s="43">
-        <f t="shared" si="11"/>
+      <c r="V5" s="41">
+        <f t="shared" si="6"/>
         <v>26.30809690259354</v>
       </c>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="40">
-        <f>Y4+1</f>
+      <c r="W5" s="25"/>
+      <c r="X5" s="38">
+        <f>X4+1</f>
         <v>5</v>
       </c>
-      <c r="Z5" s="34">
-        <f t="shared" si="12"/>
+      <c r="Y5" s="32">
+        <f>V5/D5</f>
         <v>1.3341772151898736</v>
       </c>
-      <c r="AA5" s="34">
-        <f t="shared" ref="AA5:AA13" si="16">Z5</f>
+      <c r="Z5" s="32">
+        <f t="shared" ref="Z5:Z13" si="8">Y5</f>
         <v>1.3341772151898736</v>
       </c>
-      <c r="AB5" s="47"/>
-      <c r="AC5" s="48">
-        <f t="shared" si="13"/>
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="46">
+        <f>D5*Z5</f>
         <v>26.308096902593544</v>
       </c>
+      <c r="AC5" s="15"/>
       <c r="AD5" s="15"/>
       <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-    </row>
-    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="35">
+    </row>
+    <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="33">
         <v>913</v>
       </c>
-      <c r="C6" s="36">
-        <f t="shared" si="14"/>
+      <c r="C6" s="34">
+        <f t="shared" si="7"/>
         <v>2549183</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="35">
         <v>35.815396540774046</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="32">
         <v>0.36</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="37">
         <f t="shared" si="0"/>
-        <v>917705.88</v>
-      </c>
-      <c r="G6" s="27">
-        <v>1801910.66</v>
-      </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="39">
+        <v>68.875762578411624</v>
+      </c>
+      <c r="I6" s="37">
+        <f>D6/(I$1*E6+(1-E6))</f>
+        <v>17.218940644602906</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26" t="e">
+        <f>H6*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L6" s="26" t="e">
+        <f>I6*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M6" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>68.875762578411624</v>
-      </c>
-      <c r="J6" s="39">
-        <f t="shared" si="2"/>
-        <v>17.218940644602906</v>
-      </c>
-      <c r="K6" s="25"/>
-      <c r="L6" s="26">
-        <f t="shared" ref="L6:M6" si="17">I6*F6/100000</f>
-        <v>632.07692307692309</v>
-      </c>
-      <c r="M6" s="26">
-        <f t="shared" si="17"/>
-        <v>310.26992701417242</v>
-      </c>
-      <c r="N6" s="26">
-        <f t="shared" si="4"/>
-        <v>942.34685009109558</v>
-      </c>
-      <c r="O6" s="28">
-        <f t="shared" si="5"/>
-        <v>36.966622250779778</v>
-      </c>
-      <c r="P6" s="28">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q6" s="41">
+        <v>#REF!</v>
+      </c>
+      <c r="N6" s="28" t="e">
+        <f>(H6*(#REF!/C6))+(I6*(#REF!/C6))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O6" s="28"/>
+      <c r="P6" s="39">
         <f>0.5241</f>
         <v>0.52410000000000001</v>
       </c>
-      <c r="R6" s="42">
+      <c r="Q6" s="40">
         <v>529822</v>
       </c>
-      <c r="S6" s="40">
-        <f t="shared" si="7"/>
+      <c r="R6" s="38">
+        <f t="shared" si="2"/>
         <v>277679.71020000003</v>
       </c>
-      <c r="T6" s="40">
+      <c r="S6" s="38">
+        <f t="shared" si="3"/>
+        <v>252142.28979999997</v>
+      </c>
+      <c r="T6" s="41">
+        <f t="shared" si="4"/>
+        <v>191.25401792577344</v>
+      </c>
+      <c r="U6" s="41">
+        <f t="shared" si="5"/>
+        <v>43.416231220604637</v>
+      </c>
+      <c r="V6" s="41">
+        <f t="shared" si="6"/>
+        <v>44.29228102011205</v>
+      </c>
+      <c r="W6" s="25"/>
+      <c r="X6" s="38">
+        <f>X5+1</f>
+        <v>6</v>
+      </c>
+      <c r="Y6" s="32">
+        <f>V6/D6</f>
+        <v>1.2366826923076921</v>
+      </c>
+      <c r="Z6" s="32">
         <f t="shared" si="8"/>
-        <v>252142.28979999997</v>
-      </c>
-      <c r="U6" s="43">
-        <f t="shared" si="9"/>
-        <v>191.25401792577344</v>
-      </c>
-      <c r="V6" s="43">
-        <f t="shared" si="10"/>
-        <v>43.416231220604637</v>
-      </c>
-      <c r="W6" s="43">
-        <f t="shared" si="11"/>
+        <v>1.2366826923076921</v>
+      </c>
+      <c r="AA6" s="45"/>
+      <c r="AB6" s="46">
+        <f>D6*Z6</f>
         <v>44.29228102011205</v>
       </c>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="40">
-        <f>Y5+1</f>
-        <v>6</v>
-      </c>
-      <c r="Z6" s="34">
-        <f t="shared" si="12"/>
-        <v>1.2366826923076921</v>
-      </c>
-      <c r="AA6" s="34">
-        <f t="shared" si="16"/>
-        <v>1.2366826923076921</v>
-      </c>
-      <c r="AB6" s="47"/>
-      <c r="AC6" s="48">
-        <f t="shared" si="13"/>
-        <v>44.29228102011205</v>
-      </c>
+      <c r="AC6" s="15"/>
       <c r="AD6" s="15"/>
       <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-    </row>
-    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="35">
+    </row>
+    <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="33">
         <v>1310</v>
       </c>
-      <c r="C7" s="36">
-        <f t="shared" si="14"/>
+      <c r="C7" s="34">
+        <f t="shared" si="7"/>
         <v>2437030</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="35">
         <v>53.753954608683522</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>0.36</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="37">
         <f t="shared" si="0"/>
-        <v>877330.79999999993</v>
-      </c>
-      <c r="G7" s="27">
-        <v>1275394.5600000001</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="39">
+        <v>103.37298963208369</v>
+      </c>
+      <c r="I7" s="37">
+        <f>D7/(I$1*E7+(1-E7))</f>
+        <v>25.843247408020922</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26" t="e">
+        <f>H7*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L7" s="26" t="e">
+        <f>I7*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M7" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>103.37298963208369</v>
-      </c>
-      <c r="J7" s="39">
-        <f t="shared" si="2"/>
-        <v>25.843247408020922</v>
-      </c>
-      <c r="K7" s="25"/>
-      <c r="L7" s="26">
-        <f t="shared" ref="L7:M7" si="18">I7*F7/100000</f>
-        <v>906.92307692307679</v>
-      </c>
-      <c r="M7" s="26">
-        <f t="shared" si="18"/>
-        <v>329.60337156923987</v>
-      </c>
-      <c r="N7" s="26">
-        <f t="shared" si="4"/>
-        <v>1236.5264484923166</v>
-      </c>
-      <c r="O7" s="28">
-        <f t="shared" si="5"/>
-        <v>50.739073728773</v>
-      </c>
-      <c r="P7" s="28">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q7" s="41">
+        <v>#REF!</v>
+      </c>
+      <c r="N7" s="28" t="e">
+        <f>(H7*(#REF!/C7))+(I7*(#REF!/C7))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O7" s="28"/>
+      <c r="P7" s="39">
         <f>0.6309</f>
         <v>0.63090000000000002</v>
       </c>
-      <c r="R7" s="42">
+      <c r="Q7" s="40">
         <v>446915</v>
       </c>
-      <c r="S7" s="40">
-        <f t="shared" si="7"/>
+      <c r="R7" s="38">
+        <f t="shared" si="2"/>
         <v>281958.67350000003</v>
       </c>
-      <c r="T7" s="40">
+      <c r="S7" s="38">
+        <f t="shared" si="3"/>
+        <v>164956.32649999997</v>
+      </c>
+      <c r="T7" s="41">
+        <f t="shared" si="4"/>
+        <v>291.46911032391574</v>
+      </c>
+      <c r="U7" s="41">
+        <f t="shared" si="5"/>
+        <v>42.630071572577769</v>
+      </c>
+      <c r="V7" s="41">
+        <f t="shared" si="6"/>
+        <v>74.756761777182135</v>
+      </c>
+      <c r="W7" s="25"/>
+      <c r="X7" s="38">
+        <f t="shared" ref="X7:X16" si="9">X6+1</f>
+        <v>7</v>
+      </c>
+      <c r="Y7" s="32">
+        <f>V7/D7</f>
+        <v>1.3907211538461539</v>
+      </c>
+      <c r="Z7" s="32">
         <f t="shared" si="8"/>
-        <v>164956.32649999997</v>
-      </c>
-      <c r="U7" s="43">
-        <f t="shared" si="9"/>
-        <v>291.46911032391574</v>
-      </c>
-      <c r="V7" s="43">
-        <f t="shared" si="10"/>
-        <v>42.630071572577769</v>
-      </c>
-      <c r="W7" s="43">
-        <f t="shared" si="11"/>
+        <v>1.3907211538461539</v>
+      </c>
+      <c r="AA7" s="45">
+        <f>AVERAGE(Y7:Y10)</f>
+        <v>1.4018326814868265</v>
+      </c>
+      <c r="AB7" s="46">
+        <f>D7*Z7</f>
         <v>74.756761777182135</v>
       </c>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="40">
-        <f t="shared" ref="Y7:Y16" si="19">Y6+1</f>
-        <v>7</v>
-      </c>
-      <c r="Z7" s="34">
-        <f t="shared" si="12"/>
-        <v>1.3907211538461539</v>
-      </c>
-      <c r="AA7" s="34">
-        <f t="shared" si="16"/>
-        <v>1.3907211538461539</v>
-      </c>
-      <c r="AB7" s="47">
-        <f>AVERAGE(Z7:Z10)</f>
-        <v>1.4018326814868265</v>
-      </c>
-      <c r="AC7" s="48">
-        <f t="shared" si="13"/>
-        <v>74.756761777182135</v>
-      </c>
+      <c r="AC7" s="15"/>
       <c r="AD7" s="15"/>
       <c r="AE7" s="15"/>
-      <c r="AF7" s="15"/>
-    </row>
-    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="35">
+    </row>
+    <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="33">
         <v>1501</v>
       </c>
-      <c r="C8" s="36">
-        <f t="shared" si="14"/>
+      <c r="C8" s="34">
+        <f t="shared" si="7"/>
         <v>2108701</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="35">
         <v>71.181262777416052</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>0.40300000000000002</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="37">
         <f t="shared" si="0"/>
-        <v>849806.50300000003</v>
-      </c>
-      <c r="G8" s="27">
-        <v>1202759.2799999998</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="39">
+        <v>128.89318746476422</v>
+      </c>
+      <c r="I8" s="37">
+        <f>D8/(I$1*E8+(1-E8))</f>
+        <v>32.223296866191056</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26" t="e">
+        <f>H8*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L8" s="26" t="e">
+        <f>I8*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M8" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>128.89318746476422</v>
-      </c>
-      <c r="J8" s="39">
-        <f t="shared" si="2"/>
-        <v>32.223296866191056</v>
-      </c>
-      <c r="K8" s="25"/>
-      <c r="L8" s="26">
-        <f t="shared" ref="L8:M8" si="20">I8*F8/100000</f>
-        <v>1095.3426889995471</v>
-      </c>
-      <c r="M8" s="26">
-        <f t="shared" si="20"/>
-        <v>387.56869338006209</v>
-      </c>
-      <c r="N8" s="26">
-        <f t="shared" si="4"/>
-        <v>1482.9113823796092</v>
-      </c>
-      <c r="O8" s="28">
-        <f t="shared" si="5"/>
-        <v>70.323454220375922</v>
-      </c>
-      <c r="P8" s="28">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q8" s="41">
+        <v>#REF!</v>
+      </c>
+      <c r="N8" s="28" t="e">
+        <f>(H8*(#REF!/C8))+(I8*(#REF!/C8))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O8" s="28"/>
+      <c r="P8" s="39">
         <f>0.6695</f>
         <v>0.66949999999999998</v>
       </c>
-      <c r="R8" s="42">
+      <c r="Q8" s="40">
         <v>348503</v>
       </c>
-      <c r="S8" s="40">
-        <f t="shared" si="7"/>
+      <c r="R8" s="38">
+        <f t="shared" si="2"/>
         <v>233322.7585</v>
       </c>
-      <c r="T8" s="40">
+      <c r="S8" s="38">
+        <f t="shared" si="3"/>
+        <v>115180.2415</v>
+      </c>
+      <c r="T8" s="41">
+        <f t="shared" si="4"/>
+        <v>300.73714051136409</v>
+      </c>
+      <c r="U8" s="41">
+        <f t="shared" si="5"/>
+        <v>37.114871149740793</v>
+      </c>
+      <c r="V8" s="41">
+        <f t="shared" si="6"/>
+        <v>96.943788621935781</v>
+      </c>
+      <c r="W8" s="25"/>
+      <c r="X8" s="38">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="Y8" s="32">
+        <f>V8/D8</f>
+        <v>1.3619284744228155</v>
+      </c>
+      <c r="Z8" s="32">
         <f t="shared" si="8"/>
-        <v>115180.2415</v>
-      </c>
-      <c r="U8" s="43">
-        <f t="shared" si="9"/>
-        <v>300.73714051136409</v>
-      </c>
-      <c r="V8" s="43">
-        <f t="shared" si="10"/>
-        <v>37.114871149740793</v>
-      </c>
-      <c r="W8" s="43">
-        <f t="shared" si="11"/>
+        <v>1.3619284744228155</v>
+      </c>
+      <c r="AA8" s="45"/>
+      <c r="AB8" s="46">
+        <f>D8*Z8</f>
         <v>96.943788621935781</v>
       </c>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="40">
-        <f t="shared" si="19"/>
-        <v>8</v>
-      </c>
-      <c r="Z8" s="34">
-        <f t="shared" si="12"/>
-        <v>1.3619284744228155</v>
-      </c>
-      <c r="AA8" s="34">
-        <f t="shared" si="16"/>
-        <v>1.3619284744228155</v>
-      </c>
-      <c r="AB8" s="47"/>
-      <c r="AC8" s="48">
-        <f t="shared" si="13"/>
-        <v>96.943788621935781</v>
-      </c>
+      <c r="AC8" s="15"/>
       <c r="AD8" s="15"/>
       <c r="AE8" s="15"/>
-      <c r="AF8" s="15"/>
-    </row>
-    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="35">
+    </row>
+    <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="33">
         <v>1511</v>
       </c>
-      <c r="C9" s="36">
-        <f t="shared" si="14"/>
+      <c r="C9" s="34">
+        <f t="shared" si="7"/>
         <v>1775756</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="35">
         <v>85.090519192952186</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="32">
         <v>0.40300000000000002</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="37">
         <f t="shared" si="0"/>
-        <v>715629.66800000006</v>
-      </c>
-      <c r="G9" s="27">
-        <v>1113329.52</v>
-      </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="39">
+        <v>154.07970881476177</v>
+      </c>
+      <c r="I9" s="37">
+        <f>D9/(I$1*E9+(1-E9))</f>
+        <v>38.519927203690443</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26" t="e">
+        <f>H9*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L9" s="26" t="e">
+        <f>I9*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M9" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>154.07970881476177</v>
-      </c>
-      <c r="J9" s="39">
-        <f t="shared" si="2"/>
-        <v>38.519927203690443</v>
-      </c>
-      <c r="K9" s="25"/>
-      <c r="L9" s="26">
-        <f t="shared" ref="L9:M9" si="21">I9*F9/100000</f>
-        <v>1102.6401086464464</v>
-      </c>
-      <c r="M9" s="26">
-        <f t="shared" si="21"/>
-        <v>428.85372064119622</v>
-      </c>
-      <c r="N9" s="26">
-        <f t="shared" si="4"/>
-        <v>1531.4938292876427</v>
-      </c>
-      <c r="O9" s="28">
-        <f t="shared" si="5"/>
-        <v>86.244609579674389</v>
-      </c>
-      <c r="P9" s="28">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q9" s="41">
+        <v>#REF!</v>
+      </c>
+      <c r="N9" s="28" t="e">
+        <f>(H9*(#REF!/C9))+(I9*(#REF!/C9))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O9" s="28"/>
+      <c r="P9" s="39">
         <f>0.6128</f>
         <v>0.61280000000000001</v>
       </c>
-      <c r="R9" s="42">
+      <c r="Q9" s="40">
         <v>282350</v>
       </c>
-      <c r="S9" s="40">
-        <f t="shared" si="7"/>
+      <c r="R9" s="38">
+        <f t="shared" si="2"/>
         <v>173024.08000000002</v>
       </c>
-      <c r="T9" s="40">
+      <c r="S9" s="38">
+        <f t="shared" si="3"/>
+        <v>109325.91999999998</v>
+      </c>
+      <c r="T9" s="41">
+        <f t="shared" si="4"/>
+        <v>266.59499864342047</v>
+      </c>
+      <c r="U9" s="41">
+        <f t="shared" si="5"/>
+        <v>42.112264798764848</v>
+      </c>
+      <c r="V9" s="41">
+        <f t="shared" si="6"/>
+        <v>109.33496137495494</v>
+      </c>
+      <c r="W9" s="25"/>
+      <c r="X9" s="38">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="Y9" s="32">
+        <f>V9/D9</f>
+        <v>1.2849253055681302</v>
+      </c>
+      <c r="Z9" s="32">
         <f t="shared" si="8"/>
-        <v>109325.91999999998</v>
-      </c>
-      <c r="U9" s="43">
-        <f t="shared" si="9"/>
-        <v>266.59499864342047</v>
-      </c>
-      <c r="V9" s="43">
-        <f t="shared" si="10"/>
-        <v>42.112264798764848</v>
-      </c>
-      <c r="W9" s="43">
-        <f t="shared" si="11"/>
+        <v>1.2849253055681302</v>
+      </c>
+      <c r="AA9" s="45"/>
+      <c r="AB9" s="46">
+        <f>D9*Z9</f>
         <v>109.33496137495494</v>
       </c>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="40">
-        <f t="shared" si="19"/>
-        <v>9</v>
-      </c>
-      <c r="Z9" s="34">
-        <f t="shared" si="12"/>
-        <v>1.2849253055681302</v>
-      </c>
-      <c r="AA9" s="34">
-        <f t="shared" si="16"/>
-        <v>1.2849253055681302</v>
-      </c>
-      <c r="AB9" s="47"/>
-      <c r="AC9" s="48">
-        <f t="shared" si="13"/>
-        <v>109.33496137495494</v>
-      </c>
+      <c r="AC9" s="15"/>
       <c r="AD9" s="15"/>
       <c r="AE9" s="15"/>
-      <c r="AF9" s="15"/>
-    </row>
-    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="35">
+    </row>
+    <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="33">
         <v>1498</v>
       </c>
-      <c r="C10" s="36">
-        <f t="shared" si="14"/>
+      <c r="C10" s="34">
+        <f t="shared" si="7"/>
         <v>1569513</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="35">
         <v>95.443618498222065</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="37">
         <f t="shared" si="0"/>
-        <v>312333.087</v>
-      </c>
-      <c r="G10" s="27">
-        <v>1143908.0290000001</v>
-      </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="39">
+        <v>239.05727864301082</v>
+      </c>
+      <c r="I10" s="37">
+        <f>D10/(I$1*E10+(1-E10))</f>
+        <v>59.764319660752705</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26" t="e">
+        <f>H10*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L10" s="26" t="e">
+        <f>I10*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M10" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>239.05727864301082</v>
-      </c>
-      <c r="J10" s="39">
-        <f t="shared" si="2"/>
-        <v>59.764319660752705</v>
-      </c>
-      <c r="K10" s="25"/>
-      <c r="L10" s="26">
-        <f t="shared" ref="L10:M10" si="22">I10*F10/100000</f>
-        <v>746.65497808390739</v>
-      </c>
-      <c r="M10" s="26">
-        <f t="shared" si="22"/>
-        <v>683.64885107657585</v>
-      </c>
-      <c r="N10" s="26">
-        <f t="shared" si="4"/>
-        <v>1430.3038291604832</v>
-      </c>
-      <c r="O10" s="28">
-        <f t="shared" si="5"/>
-        <v>91.130422568050292</v>
-      </c>
-      <c r="P10" s="28">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q10" s="41">
+        <v>#REF!</v>
+      </c>
+      <c r="N10" s="28" t="e">
+        <f>(H10*(#REF!/C10))+(I10*(#REF!/C10))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O10" s="28"/>
+      <c r="P10" s="39">
         <f>0.5023</f>
         <v>0.50229999999999997</v>
       </c>
-      <c r="R10" s="42">
+      <c r="Q10" s="40">
         <v>243989</v>
       </c>
-      <c r="S10" s="40">
-        <f t="shared" si="7"/>
+      <c r="R10" s="38">
+        <f t="shared" si="2"/>
         <v>122555.67469999999</v>
       </c>
-      <c r="T10" s="40">
+      <c r="S10" s="38">
+        <f t="shared" si="3"/>
+        <v>121433.32530000001</v>
+      </c>
+      <c r="T10" s="41">
+        <f t="shared" si="4"/>
+        <v>292.97826076040087</v>
+      </c>
+      <c r="U10" s="41">
+        <f t="shared" si="5"/>
+        <v>72.573800706973685</v>
+      </c>
+      <c r="V10" s="41">
+        <f t="shared" si="6"/>
+        <v>149.82317295754092</v>
+      </c>
+      <c r="W10" s="25"/>
+      <c r="X10" s="38">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="Y10" s="32">
+        <f>V10/D10</f>
+        <v>1.5697557921102063</v>
+      </c>
+      <c r="Z10" s="32">
         <f t="shared" si="8"/>
-        <v>121433.32530000001</v>
-      </c>
-      <c r="U10" s="43">
-        <f t="shared" si="9"/>
-        <v>292.97826076040087</v>
-      </c>
-      <c r="V10" s="43">
-        <f t="shared" si="10"/>
-        <v>72.573800706973685</v>
-      </c>
-      <c r="W10" s="43">
-        <f t="shared" si="11"/>
+        <v>1.5697557921102063</v>
+      </c>
+      <c r="AA10" s="45"/>
+      <c r="AB10" s="46">
+        <f>D10*Z10</f>
         <v>149.82317295754092</v>
       </c>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="40">
-        <f t="shared" si="19"/>
-        <v>10</v>
-      </c>
-      <c r="Z10" s="34">
-        <f t="shared" si="12"/>
-        <v>1.5697557921102063</v>
-      </c>
-      <c r="AA10" s="34">
-        <f t="shared" si="16"/>
-        <v>1.5697557921102063</v>
-      </c>
-      <c r="AB10" s="47"/>
-      <c r="AC10" s="48">
-        <f t="shared" si="13"/>
-        <v>149.82317295754092</v>
-      </c>
+      <c r="AC10" s="15"/>
       <c r="AD10" s="15"/>
       <c r="AE10" s="15"/>
-      <c r="AF10" s="15"/>
-    </row>
-    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="35">
+    </row>
+    <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="33">
         <v>1320</v>
       </c>
-      <c r="C11" s="36">
-        <f t="shared" si="14"/>
+      <c r="C11" s="34">
+        <f t="shared" si="7"/>
         <v>1373576.0000000002</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="35">
         <v>96.099524161750054</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="32">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="37">
         <f t="shared" si="0"/>
-        <v>273341.62400000007</v>
-      </c>
-      <c r="G11" s="27">
-        <v>1028312.88</v>
-      </c>
-      <c r="H11" s="25"/>
-      <c r="I11" s="39">
+        <v>240.70012313525373</v>
+      </c>
+      <c r="I11" s="37">
+        <f>D11/(I$1*E11+(1-E11))</f>
+        <v>60.175030783813433</v>
+      </c>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26" t="e">
+        <f>H11*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L11" s="26" t="e">
+        <f>I11*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M11" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>240.70012313525373</v>
-      </c>
-      <c r="J11" s="39">
+        <v>#REF!</v>
+      </c>
+      <c r="N11" s="28" t="e">
+        <f>(H11*(#REF!/C11))+(I11*(#REF!/C11))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O11" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="39">
+        <f t="shared" ref="P11:P16" si="10">0.5023</f>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q11" s="40">
+        <v>216352</v>
+      </c>
+      <c r="R11" s="38">
         <f t="shared" si="2"/>
-        <v>60.175030783813433</v>
-      </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="26">
-        <f t="shared" ref="L11:M11" si="23">I11*F11/100000</f>
-        <v>657.93362554790247</v>
-      </c>
-      <c r="M11" s="26">
-        <f t="shared" si="23"/>
-        <v>618.78759209391842</v>
-      </c>
-      <c r="N11" s="26">
+        <v>108673.6096</v>
+      </c>
+      <c r="S11" s="38">
+        <f t="shared" si="3"/>
+        <v>107678.3904</v>
+      </c>
+      <c r="T11" s="41">
         <f t="shared" si="4"/>
-        <v>1276.7212176418209</v>
-      </c>
-      <c r="O11" s="28">
+        <v>261.5775121227249</v>
+      </c>
+      <c r="U11" s="41">
         <f t="shared" si="5"/>
-        <v>92.9487132595372</v>
-      </c>
-      <c r="P11" s="28">
+        <v>64.795504570714812</v>
+      </c>
+      <c r="V11" s="41">
         <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q11" s="41">
-        <f t="shared" ref="Q11:Q16" si="24">0.5023</f>
-        <v>0.50229999999999997</v>
-      </c>
-      <c r="R11" s="42">
-        <v>216352</v>
-      </c>
-      <c r="S11" s="40">
-        <f t="shared" si="7"/>
-        <v>108673.6096</v>
-      </c>
-      <c r="T11" s="40">
+        <v>150.85278467194186</v>
+      </c>
+      <c r="W11" s="25"/>
+      <c r="X11" s="38">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="Y11" s="32">
+        <f>V11/D11</f>
+        <v>1.5697557921102063</v>
+      </c>
+      <c r="Z11" s="32">
         <f t="shared" si="8"/>
-        <v>107678.3904</v>
-      </c>
-      <c r="U11" s="43">
-        <f t="shared" si="9"/>
-        <v>261.5775121227249</v>
-      </c>
-      <c r="V11" s="43">
-        <f t="shared" si="10"/>
-        <v>64.795504570714812</v>
-      </c>
-      <c r="W11" s="43">
-        <f t="shared" si="11"/>
+        <v>1.5697557921102063</v>
+      </c>
+      <c r="AA11" s="45">
+        <f>AVERAGE(Y11:Y13)</f>
+        <v>1.5677935973700687</v>
+      </c>
+      <c r="AB11" s="46">
+        <f>D11*Z11</f>
         <v>150.85278467194186</v>
       </c>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="40">
-        <f t="shared" si="19"/>
-        <v>11</v>
-      </c>
-      <c r="Z11" s="34">
-        <f t="shared" si="12"/>
-        <v>1.5697557921102063</v>
-      </c>
-      <c r="AA11" s="34">
-        <f t="shared" si="16"/>
-        <v>1.5697557921102063</v>
-      </c>
-      <c r="AB11" s="47">
-        <f>AVERAGE(Z11:Z13)</f>
-        <v>1.5677935973700687</v>
-      </c>
-      <c r="AC11" s="48">
-        <f t="shared" si="13"/>
-        <v>150.85278467194186</v>
-      </c>
+      <c r="AC11" s="15"/>
       <c r="AD11" s="15"/>
       <c r="AE11" s="15"/>
-      <c r="AF11" s="15"/>
-    </row>
-    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="35">
+    </row>
+    <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="33">
         <v>1123</v>
       </c>
-      <c r="C12" s="36">
-        <f t="shared" si="14"/>
+      <c r="C12" s="34">
+        <f t="shared" si="7"/>
         <v>1183955</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="35">
         <v>94.851577973825016</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="32">
         <v>0.2</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="37">
         <f t="shared" si="0"/>
-        <v>236791</v>
-      </c>
-      <c r="G12" s="27">
-        <v>889868.57400000002</v>
-      </c>
-      <c r="H12" s="25"/>
-      <c r="I12" s="39">
+        <v>237.12894493456253</v>
+      </c>
+      <c r="I12" s="37">
+        <f>D12/(I$1*E12+(1-E12))</f>
+        <v>59.282236233640631</v>
+      </c>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26" t="e">
+        <f>H12*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L12" s="26" t="e">
+        <f>I12*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M12" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>237.12894493456253</v>
-      </c>
-      <c r="J12" s="39">
+        <v>#REF!</v>
+      </c>
+      <c r="N12" s="28" t="e">
+        <f>(H12*(#REF!/C12))+(I12*(#REF!/C12))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O12" s="57"/>
+      <c r="P12" s="39">
+        <f t="shared" si="10"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q12" s="40">
+        <v>189489</v>
+      </c>
+      <c r="R12" s="38">
         <f t="shared" si="2"/>
-        <v>59.282236233640631</v>
-      </c>
-      <c r="K12" s="25"/>
-      <c r="L12" s="26">
-        <f t="shared" ref="L12:M12" si="25">I12*F12/100000</f>
-        <v>561.49999999999989</v>
-      </c>
-      <c r="M12" s="26">
-        <f t="shared" si="25"/>
-        <v>527.53399020760924</v>
-      </c>
-      <c r="N12" s="26">
+        <v>95180.324699999997</v>
+      </c>
+      <c r="S12" s="38">
+        <f t="shared" si="3"/>
+        <v>94308.675300000003</v>
+      </c>
+      <c r="T12" s="41">
         <f t="shared" si="4"/>
-        <v>1089.0339902076091</v>
-      </c>
-      <c r="O12" s="28">
+        <v>225.70009974640084</v>
+      </c>
+      <c r="U12" s="41">
         <f t="shared" si="5"/>
-        <v>91.982718110706003</v>
-      </c>
-      <c r="P12" s="28">
+        <v>55.908291680163096</v>
+      </c>
+      <c r="V12" s="41">
         <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q12" s="41">
-        <f t="shared" si="24"/>
-        <v>0.50229999999999997</v>
-      </c>
-      <c r="R12" s="42">
-        <v>189489</v>
-      </c>
-      <c r="S12" s="40">
-        <f t="shared" si="7"/>
-        <v>95180.324699999997</v>
-      </c>
-      <c r="T12" s="40">
+        <v>148.61463801411369</v>
+      </c>
+      <c r="W12" s="25"/>
+      <c r="X12" s="38">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="Y12" s="32">
+        <f>V12/D12</f>
+        <v>1.5668124999999999</v>
+      </c>
+      <c r="Z12" s="32">
         <f t="shared" si="8"/>
-        <v>94308.675300000003</v>
-      </c>
-      <c r="U12" s="43">
-        <f t="shared" si="9"/>
-        <v>225.70009974640084</v>
-      </c>
-      <c r="V12" s="43">
-        <f t="shared" si="10"/>
-        <v>55.908291680163096</v>
-      </c>
-      <c r="W12" s="43">
-        <f t="shared" si="11"/>
+        <v>1.5668124999999999</v>
+      </c>
+      <c r="AA12" s="45"/>
+      <c r="AB12" s="46">
+        <f>D12*Z12</f>
         <v>148.61463801411369</v>
       </c>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="40">
-        <f t="shared" si="19"/>
-        <v>12</v>
-      </c>
-      <c r="Z12" s="34">
-        <f t="shared" si="12"/>
-        <v>1.5668124999999999</v>
-      </c>
-      <c r="AA12" s="34">
-        <f t="shared" si="16"/>
-        <v>1.5668124999999999</v>
-      </c>
-      <c r="AB12" s="47"/>
-      <c r="AC12" s="48">
-        <f t="shared" si="13"/>
-        <v>148.61463801411369</v>
-      </c>
+      <c r="AC12" s="15"/>
       <c r="AD12" s="15"/>
       <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
-    </row>
-    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="35">
+    </row>
+    <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="33">
         <v>966</v>
       </c>
-      <c r="C13" s="36">
-        <f t="shared" si="14"/>
+      <c r="C13" s="34">
+        <f t="shared" si="7"/>
         <v>990896</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="35">
         <v>97.48752644071628</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="32">
         <v>0.2</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="37">
         <f t="shared" si="0"/>
-        <v>198179.20000000001</v>
-      </c>
-      <c r="G13" s="27">
-        <v>754842.304</v>
-      </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="39">
+        <v>243.71881610179068</v>
+      </c>
+      <c r="I13" s="37">
+        <f>D13/(I$1*E13+(1-E13))</f>
+        <v>60.92970402544767</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26" t="e">
+        <f>H13*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L13" s="26" t="e">
+        <f>I13*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M13" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>243.71881610179068</v>
-      </c>
-      <c r="J13" s="39">
+        <v>#REF!</v>
+      </c>
+      <c r="N13" s="28" t="e">
+        <f>(H13*(#REF!/C13))+(I13*(#REF!/C13))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O13" s="57"/>
+      <c r="P13" s="39">
+        <f t="shared" si="10"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q13" s="40">
+        <v>163816</v>
+      </c>
+      <c r="R13" s="38">
         <f t="shared" si="2"/>
-        <v>60.92970402544767</v>
-      </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="26">
-        <f t="shared" ref="L13:M13" si="26">I13*F13/100000</f>
-        <v>483</v>
-      </c>
-      <c r="M13" s="26">
-        <f t="shared" si="26"/>
-        <v>459.92318168606994</v>
-      </c>
-      <c r="N13" s="26">
+        <v>82284.776799999992</v>
+      </c>
+      <c r="S13" s="38">
+        <f t="shared" si="3"/>
+        <v>81531.223200000008</v>
+      </c>
+      <c r="T13" s="41">
         <f t="shared" si="4"/>
-        <v>942.92318168606994</v>
-      </c>
-      <c r="O13" s="28">
+        <v>200.54348384896093</v>
+      </c>
+      <c r="U13" s="41">
         <f t="shared" si="5"/>
-        <v>95.158642449466953</v>
-      </c>
-      <c r="P13" s="28">
+        <v>49.676732984087131</v>
+      </c>
+      <c r="V13" s="41">
         <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q13" s="41">
-        <f t="shared" si="24"/>
-        <v>0.50229999999999997</v>
-      </c>
-      <c r="R13" s="42">
-        <v>163816</v>
-      </c>
-      <c r="S13" s="40">
-        <f t="shared" si="7"/>
-        <v>82284.776799999992</v>
-      </c>
-      <c r="T13" s="40">
+        <v>152.74467502139476</v>
+      </c>
+      <c r="W13" s="25"/>
+      <c r="X13" s="38">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="Y13" s="32">
+        <f>V13/D13</f>
+        <v>1.5668124999999997</v>
+      </c>
+      <c r="Z13" s="32">
         <f t="shared" si="8"/>
-        <v>81531.223200000008</v>
-      </c>
-      <c r="U13" s="43">
-        <f t="shared" si="9"/>
-        <v>200.54348384896093</v>
-      </c>
-      <c r="V13" s="43">
-        <f t="shared" si="10"/>
-        <v>49.676732984087131</v>
-      </c>
-      <c r="W13" s="43">
-        <f t="shared" si="11"/>
+        <v>1.5668124999999997</v>
+      </c>
+      <c r="AA13" s="45"/>
+      <c r="AB13" s="46">
+        <f>D13*Z13</f>
         <v>152.74467502139476</v>
       </c>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="40">
-        <f t="shared" si="19"/>
-        <v>13</v>
-      </c>
-      <c r="Z13" s="34">
-        <f t="shared" si="12"/>
-        <v>1.5668124999999997</v>
-      </c>
-      <c r="AA13" s="34">
-        <f t="shared" si="16"/>
-        <v>1.5668124999999997</v>
-      </c>
-      <c r="AB13" s="47"/>
-      <c r="AC13" s="48">
-        <f t="shared" si="13"/>
-        <v>152.74467502139476</v>
-      </c>
+      <c r="AC13" s="15"/>
       <c r="AD13" s="15"/>
       <c r="AE13" s="15"/>
-      <c r="AF13" s="15"/>
-    </row>
-    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="35">
+    </row>
+    <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="33">
         <v>766</v>
       </c>
-      <c r="C14" s="36">
-        <f t="shared" si="14"/>
+      <c r="C14" s="34">
+        <f t="shared" si="7"/>
         <v>751066.99999999988</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="35">
         <v>101.98823806664386</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="32">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="37">
         <f t="shared" si="0"/>
-        <v>39806.550999999992</v>
-      </c>
-      <c r="G14" s="27">
-        <v>542905.85600000003</v>
-      </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="39">
+        <v>351.98701662344729</v>
+      </c>
+      <c r="I14" s="37">
+        <f>D14/(I$1*E14+(1-E14))</f>
+        <v>87.996754155861822</v>
+      </c>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26" t="e">
+        <f>H14*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L14" s="26" t="e">
+        <f>I14*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M14" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>351.98701662344729</v>
-      </c>
-      <c r="J14" s="39">
+        <v>#REF!</v>
+      </c>
+      <c r="N14" s="28" t="e">
+        <f>(H14*(#REF!/C14))+(I14*(#REF!/C14))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O14" s="57"/>
+      <c r="P14" s="39">
+        <f t="shared" si="10"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q14" s="40">
+        <v>134732</v>
+      </c>
+      <c r="R14" s="38">
         <f t="shared" si="2"/>
-        <v>87.996754155861822</v>
-      </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="26">
-        <f t="shared" ref="L14:M14" si="27">I14*F14/100000</f>
-        <v>140.113891285591</v>
-      </c>
-      <c r="M14" s="26">
-        <f t="shared" si="27"/>
-        <v>477.73953140209721</v>
-      </c>
-      <c r="N14" s="26">
+        <v>67675.883600000001</v>
+      </c>
+      <c r="S14" s="38">
+        <f t="shared" si="3"/>
+        <v>67056.116399999999</v>
+      </c>
+      <c r="T14" s="41">
         <f t="shared" si="4"/>
-        <v>617.85342268768818</v>
-      </c>
-      <c r="O14" s="28">
+        <v>238.21032365719682</v>
+      </c>
+      <c r="U14" s="41">
         <f t="shared" si="5"/>
-        <v>82.263422928671929</v>
-      </c>
-      <c r="P14" s="28">
+        <v>59.007205894976536</v>
+      </c>
+      <c r="V14" s="41">
         <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q14" s="41">
-        <f t="shared" si="24"/>
-        <v>0.50229999999999997</v>
-      </c>
-      <c r="R14" s="42">
-        <v>134732</v>
-      </c>
-      <c r="S14" s="40">
-        <f t="shared" si="7"/>
-        <v>67675.883600000001</v>
-      </c>
-      <c r="T14" s="40">
-        <f t="shared" si="8"/>
-        <v>67056.116399999999</v>
-      </c>
-      <c r="U14" s="43">
+        <v>220.59906299332997</v>
+      </c>
+      <c r="W14" s="25"/>
+      <c r="X14" s="38">
         <f t="shared" si="9"/>
-        <v>238.21032365719682</v>
-      </c>
-      <c r="V14" s="43">
-        <f t="shared" si="10"/>
-        <v>59.007205894976536</v>
-      </c>
-      <c r="W14" s="43">
-        <f t="shared" si="11"/>
-        <v>220.59906299332997</v>
-      </c>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="40">
-        <f t="shared" si="19"/>
         <v>14</v>
       </c>
-      <c r="Z14" s="34">
-        <f t="shared" si="12"/>
+      <c r="Y14" s="32">
+        <f>V14/D14</f>
         <v>2.1629853321829158</v>
       </c>
-      <c r="AA14" s="34">
-        <f>AA13</f>
+      <c r="Z14" s="32">
+        <f>Z13</f>
         <v>1.5668124999999997</v>
       </c>
-      <c r="AB14" s="47"/>
-      <c r="AC14" s="48">
-        <f t="shared" si="13"/>
+      <c r="AA14" s="45"/>
+      <c r="AB14" s="46">
+        <f>D14*Z14</f>
         <v>159.7964462557934</v>
       </c>
+      <c r="AC14" s="15"/>
       <c r="AD14" s="15"/>
       <c r="AE14" s="15"/>
-      <c r="AF14" s="15"/>
-    </row>
-    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="35">
+    </row>
+    <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="33">
         <v>562</v>
       </c>
-      <c r="C15" s="36">
-        <f t="shared" si="14"/>
+      <c r="C15" s="34">
+        <f t="shared" si="7"/>
         <v>508942</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="35">
         <v>110.42515650113373</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="32">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="37">
         <f t="shared" si="0"/>
-        <v>26973.925999999999</v>
-      </c>
-      <c r="G15" s="27">
-        <v>443916.03200000001</v>
-      </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="39">
+        <v>381.10494046983166</v>
+      </c>
+      <c r="I15" s="37">
+        <f>D15/(I$1*E15+(1-E15))</f>
+        <v>95.276235117457915</v>
+      </c>
+      <c r="J15" s="25"/>
+      <c r="K15" s="26" t="e">
+        <f>H15*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L15" s="26" t="e">
+        <f>I15*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M15" s="26" t="e">
         <f t="shared" si="1"/>
-        <v>381.10494046983166</v>
-      </c>
-      <c r="J15" s="39">
+        <v>#REF!</v>
+      </c>
+      <c r="N15" s="28" t="e">
+        <f>(H15*(#REF!/C15))+(I15*(#REF!/C15))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O15" s="57"/>
+      <c r="P15" s="39">
+        <f t="shared" si="10"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q15" s="40">
+        <v>93602</v>
+      </c>
+      <c r="R15" s="38">
         <f t="shared" si="2"/>
-        <v>95.276235117457915</v>
-      </c>
-      <c r="K15" s="25"/>
-      <c r="L15" s="26">
-        <f t="shared" ref="L15:M15" si="28">I15*F15/100000</f>
-        <v>102.79896462467644</v>
-      </c>
-      <c r="M15" s="26">
-        <f t="shared" si="28"/>
-        <v>422.94648237240972</v>
-      </c>
-      <c r="N15" s="26">
+        <v>47016.284599999999</v>
+      </c>
+      <c r="S15" s="38">
+        <f t="shared" si="3"/>
+        <v>46585.715400000001</v>
+      </c>
+      <c r="T15" s="41">
         <f t="shared" si="4"/>
-        <v>525.74544699708622</v>
-      </c>
-      <c r="O15" s="28">
+        <v>179.1813834359566</v>
+      </c>
+      <c r="U15" s="41">
         <f t="shared" si="5"/>
-        <v>103.30164281923798</v>
-      </c>
-      <c r="P15" s="28">
+        <v>44.385115735653798</v>
+      </c>
+      <c r="V15" s="41">
         <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="Q15" s="41">
-        <f t="shared" si="24"/>
-        <v>0.50229999999999997</v>
-      </c>
-      <c r="R15" s="42">
-        <v>93602</v>
-      </c>
-      <c r="S15" s="40">
-        <f t="shared" si="7"/>
-        <v>47016.284599999999</v>
-      </c>
-      <c r="T15" s="40">
-        <f t="shared" si="8"/>
-        <v>46585.715400000001</v>
-      </c>
-      <c r="U15" s="43">
+        <v>238.84799381595525</v>
+      </c>
+      <c r="W15" s="25"/>
+      <c r="X15" s="38">
         <f t="shared" si="9"/>
-        <v>179.1813834359566</v>
-      </c>
-      <c r="V15" s="43">
-        <f t="shared" si="10"/>
-        <v>44.385115735653798</v>
-      </c>
-      <c r="W15" s="43">
-        <f t="shared" si="11"/>
-        <v>238.84799381595525</v>
-      </c>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="40">
-        <f t="shared" si="19"/>
         <v>15</v>
       </c>
-      <c r="Z15" s="34">
-        <f t="shared" si="12"/>
+      <c r="Y15" s="32">
+        <f>V15/D15</f>
         <v>2.1629853321829162</v>
       </c>
-      <c r="AA15" s="34">
-        <f t="shared" ref="AA15" si="29">AA14</f>
+      <c r="Z15" s="32">
+        <f t="shared" ref="Z15" si="11">Z14</f>
         <v>1.5668124999999997</v>
       </c>
-      <c r="AB15" s="47"/>
-      <c r="AC15" s="48">
-        <f t="shared" si="13"/>
+      <c r="AA15" s="45"/>
+      <c r="AB15" s="46">
+        <f>D15*Z15</f>
         <v>173.01551552043256</v>
       </c>
+      <c r="AC15" s="15"/>
       <c r="AD15" s="15"/>
       <c r="AE15" s="15"/>
-      <c r="AF15" s="15"/>
-    </row>
-    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="35">
+    </row>
+    <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="33">
         <v>902</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="34">
+      <c r="C16" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="32">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="F16" s="27" t="e">
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="37" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G16" s="27">
-        <v>308400.38400000002</v>
-      </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="39" t="e">
+      <c r="I16" s="37" t="e">
+        <f>D16/(I$1*E16+(1-E16))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26" t="e">
+        <f>H16*#REF!/100000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L16" s="26" t="e">
+        <f>I16*#REF!/100000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M16" s="26" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J16" s="39" t="e">
+      <c r="N16" s="28" t="e">
+        <f>(H16*(#REF!/C16))+(I16*(#REF!/C16))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O16" s="57"/>
+      <c r="P16" s="39">
+        <f t="shared" si="10"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q16" s="40">
+        <v>58431</v>
+      </c>
+      <c r="R16" s="38">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K16" s="25"/>
-      <c r="L16" s="26" t="e">
-        <f t="shared" ref="L16:M16" si="30">I16*F16/100000</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M16" s="26" t="e">
-        <f t="shared" si="30"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N16" s="26" t="e">
+        <v>29349.891299999999</v>
+      </c>
+      <c r="S16" s="38">
+        <f t="shared" si="3"/>
+        <v>29081.108700000001</v>
+      </c>
+      <c r="T16" s="41" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="O16" s="28" t="e">
+      <c r="U16" s="41" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="P16" s="28" t="e">
+      <c r="V16" s="41" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q16" s="41">
-        <f t="shared" si="24"/>
-        <v>0.50229999999999997</v>
-      </c>
-      <c r="R16" s="42">
-        <v>58431</v>
-      </c>
-      <c r="S16" s="40">
-        <f t="shared" si="7"/>
-        <v>29349.891299999999</v>
-      </c>
-      <c r="T16" s="40">
-        <f t="shared" si="8"/>
-        <v>29081.108700000001</v>
-      </c>
-      <c r="U16" s="43" t="e">
+      <c r="W16" s="25"/>
+      <c r="X16" s="38">
         <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="Y16" s="32" t="e">
+        <f>V16/D16</f>
         <v>#VALUE!</v>
       </c>
-      <c r="V16" s="43" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W16" s="43" t="e">
-        <f t="shared" si="11"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="40">
-        <f t="shared" si="19"/>
-        <v>16</v>
-      </c>
-      <c r="Z16" s="34" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AA16" s="34"/>
-      <c r="AB16" s="34"/>
-      <c r="AC16" s="48"/>
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="32"/>
+      <c r="AB16" s="46"/>
+      <c r="AC16" s="15"/>
       <c r="AD16" s="15"/>
       <c r="AE16" s="15"/>
-      <c r="AF16" s="15"/>
-    </row>
-    <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -3532,19 +3472,18 @@
       <c r="X17" s="25"/>
       <c r="Y17" s="25"/>
       <c r="Z17" s="25"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="26"/>
-    </row>
-    <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA17" s="26"/>
+    </row>
+    <row r="18" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B18" s="27">
-        <f t="shared" ref="B18:C18" si="31">SUM(B4:B16)</f>
+        <f t="shared" ref="B18:C18" si="12">SUM(B4:B16)</f>
         <v>12975</v>
       </c>
       <c r="C18" s="27">
-        <f t="shared" si="31"/>
+        <f t="shared" si="12"/>
         <v>20358985</v>
       </c>
       <c r="D18" s="28">
@@ -3552,74 +3491,64 @@
         <v>63.731075002019992</v>
       </c>
       <c r="E18" s="25"/>
-      <c r="F18" s="27" t="e">
-        <f t="shared" ref="F18:G18" si="32">SUM(F4:F16)</f>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="29" t="e">
+        <f>K18/#REF!*100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I18" s="29" t="e">
+        <f>L18/#REF!*100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26" t="e">
+        <f t="shared" ref="K18:L18" si="13">SUM(K4:K16)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L18" s="26" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
+      </c>
+      <c r="M18" s="26"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="27">
+        <f t="shared" ref="Q18:U18" si="14">SUM(Q4:Q16)</f>
+        <v>3789911</v>
+      </c>
+      <c r="R18" s="26">
+        <f t="shared" si="14"/>
+        <v>1750735.6040000003</v>
+      </c>
+      <c r="S18" s="26">
+        <f t="shared" si="14"/>
+        <v>2039175.3959999997</v>
+      </c>
+      <c r="T18" s="29" t="e">
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G18" s="27">
-        <f t="shared" si="32"/>
-        <v>15083772.494999999</v>
-      </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="29" t="e">
-        <f t="shared" ref="I18:J18" si="33">L18/F18*100000</f>
+      <c r="U18" s="29" t="e">
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J18" s="29" t="e">
-        <f t="shared" si="33"/>
+      <c r="V18" s="29" t="e">
+        <f>(T18+U18)/Q18*100000</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K18" s="25"/>
-      <c r="L18" s="26" t="e">
-        <f t="shared" ref="L18:M18" si="34">SUM(L4:L16)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M18" s="26" t="e">
-        <f t="shared" si="34"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N18" s="26"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="30" t="e">
-        <f>I18/J18</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="27">
-        <f t="shared" ref="R18:V18" si="35">SUM(R4:R16)</f>
-        <v>3789911</v>
-      </c>
-      <c r="S18" s="26">
-        <f t="shared" si="35"/>
-        <v>1750735.6040000003</v>
-      </c>
-      <c r="T18" s="26">
-        <f t="shared" si="35"/>
-        <v>2039175.3959999997</v>
-      </c>
-      <c r="U18" s="29" t="e">
-        <f t="shared" si="35"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="V18" s="29" t="e">
-        <f t="shared" si="35"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="W18" s="29" t="e">
-        <f>(U18+V18)/R18*100000</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="W18" s="25"/>
       <c r="X18" s="25"/>
-      <c r="Y18" s="25"/>
+      <c r="Y18" s="27"/>
       <c r="Z18" s="27"/>
-      <c r="AA18" s="27"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="18"/>
+      <c r="AA18" s="26"/>
+      <c r="AB18" s="18"/>
+      <c r="AC18" s="15"/>
       <c r="AD18" s="15"/>
       <c r="AE18" s="15"/>
-      <c r="AF18" s="15"/>
-    </row>
-    <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
@@ -3646,44 +3575,45 @@
       <c r="X19" s="25"/>
       <c r="Y19" s="25"/>
       <c r="Z19" s="25"/>
-      <c r="AA19" s="25"/>
-      <c r="AB19" s="26"/>
-    </row>
-    <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA19" s="26"/>
+    </row>
+    <row r="20" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="AB20" s="18"/>
-    </row>
-    <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA20" s="18"/>
+    </row>
+    <row r="21" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="H21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="21"/>
-      <c r="AB21" s="18"/>
-    </row>
-    <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="21"/>
+      <c r="AA21" s="18"/>
+    </row>
+    <row r="22" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="23"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="AB22" s="18"/>
-    </row>
-    <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="AA22" s="18"/>
+    </row>
+    <row r="23" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -3695,446 +3625,417 @@
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
       <c r="V23" s="5"/>
-      <c r="W23" s="5"/>
+      <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
-      <c r="AB23" s="18"/>
+      <c r="AA23" s="18"/>
+      <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
       <c r="AD23" s="5"/>
       <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
-    </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="9"/>
       <c r="D24" s="12"/>
       <c r="E24" s="14"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
+      <c r="K24" s="16"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
+      <c r="N24" s="12"/>
       <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="5"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="18"/>
       <c r="S24" s="18"/>
-      <c r="T24" s="18"/>
+      <c r="T24" s="15"/>
       <c r="U24" s="15"/>
       <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
+      <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
-      <c r="AA24" s="5"/>
+      <c r="AA24" s="18"/>
       <c r="AB24" s="18"/>
-      <c r="AC24" s="18"/>
+      <c r="AC24" s="15"/>
       <c r="AD24" s="15"/>
       <c r="AE24" s="15"/>
-      <c r="AF24" s="15"/>
-    </row>
-    <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="9"/>
       <c r="D25" s="12"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="H25" s="12"/>
       <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
+      <c r="K25" s="16"/>
       <c r="L25" s="16"/>
       <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
+      <c r="N25" s="12"/>
       <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="5"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="18"/>
       <c r="S25" s="18"/>
-      <c r="T25" s="18"/>
+      <c r="T25" s="15"/>
       <c r="U25" s="15"/>
       <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
+      <c r="Y25" s="5"/>
       <c r="Z25" s="5"/>
-      <c r="AA25" s="5"/>
+      <c r="AA25" s="18"/>
       <c r="AB25" s="18"/>
-      <c r="AC25" s="18"/>
+      <c r="AC25" s="15"/>
       <c r="AD25" s="15"/>
       <c r="AE25" s="15"/>
-      <c r="AF25" s="15"/>
-    </row>
-    <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="9"/>
       <c r="D26" s="12"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
+      <c r="K26" s="16"/>
       <c r="L26" s="16"/>
       <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
+      <c r="N26" s="12"/>
       <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="5"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="18"/>
       <c r="S26" s="18"/>
-      <c r="T26" s="18"/>
+      <c r="T26" s="15"/>
       <c r="U26" s="15"/>
       <c r="V26" s="15"/>
-      <c r="W26" s="15"/>
+      <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
-      <c r="AA26" s="5"/>
+      <c r="AA26" s="18"/>
       <c r="AB26" s="18"/>
-      <c r="AC26" s="18"/>
+      <c r="AC26" s="15"/>
       <c r="AD26" s="15"/>
       <c r="AE26" s="15"/>
-      <c r="AF26" s="15"/>
-    </row>
-    <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="9"/>
       <c r="D27" s="12"/>
       <c r="E27" s="14"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
+      <c r="K27" s="16"/>
       <c r="L27" s="16"/>
       <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
+      <c r="N27" s="12"/>
       <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="5"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="18"/>
       <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
+      <c r="T27" s="15"/>
       <c r="U27" s="15"/>
       <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
+      <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
-      <c r="AA27" s="5"/>
+      <c r="AA27" s="18"/>
       <c r="AB27" s="18"/>
-      <c r="AC27" s="18"/>
+      <c r="AC27" s="15"/>
       <c r="AD27" s="15"/>
       <c r="AE27" s="15"/>
-      <c r="AF27" s="15"/>
-    </row>
-    <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="9"/>
       <c r="D28" s="12"/>
       <c r="E28" s="14"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
+      <c r="K28" s="16"/>
       <c r="L28" s="16"/>
       <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
+      <c r="N28" s="12"/>
       <c r="O28" s="12"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="5"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="18"/>
       <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
+      <c r="T28" s="15"/>
       <c r="U28" s="15"/>
       <c r="V28" s="15"/>
-      <c r="W28" s="15"/>
+      <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
-      <c r="AA28" s="5"/>
+      <c r="AA28" s="18"/>
       <c r="AB28" s="18"/>
-      <c r="AC28" s="18"/>
+      <c r="AC28" s="15"/>
       <c r="AD28" s="15"/>
       <c r="AE28" s="15"/>
-      <c r="AF28" s="15"/>
-    </row>
-    <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="9"/>
       <c r="D29" s="12"/>
       <c r="E29" s="14"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
+      <c r="K29" s="16"/>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
+      <c r="N29" s="12"/>
       <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="5"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="18"/>
       <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
+      <c r="T29" s="15"/>
       <c r="U29" s="15"/>
       <c r="V29" s="15"/>
-      <c r="W29" s="15"/>
+      <c r="Y29" s="5"/>
       <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
+      <c r="AA29" s="18"/>
       <c r="AB29" s="18"/>
-      <c r="AC29" s="18"/>
+      <c r="AC29" s="15"/>
       <c r="AD29" s="15"/>
       <c r="AE29" s="15"/>
-      <c r="AF29" s="15"/>
-    </row>
-    <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="9"/>
       <c r="D30" s="12"/>
       <c r="E30" s="14"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
+      <c r="K30" s="16"/>
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
+      <c r="N30" s="12"/>
       <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="5"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="18"/>
       <c r="S30" s="18"/>
-      <c r="T30" s="18"/>
+      <c r="T30" s="15"/>
       <c r="U30" s="15"/>
       <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
+      <c r="Y30" s="5"/>
       <c r="Z30" s="5"/>
-      <c r="AA30" s="5"/>
+      <c r="AA30" s="18"/>
       <c r="AB30" s="18"/>
-      <c r="AC30" s="18"/>
+      <c r="AC30" s="15"/>
       <c r="AD30" s="15"/>
       <c r="AE30" s="15"/>
-      <c r="AF30" s="15"/>
-    </row>
-    <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="9"/>
       <c r="D31" s="12"/>
       <c r="E31" s="14"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
+      <c r="K31" s="16"/>
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
-      <c r="N31" s="16"/>
+      <c r="N31" s="12"/>
       <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="5"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="18"/>
       <c r="S31" s="18"/>
-      <c r="T31" s="18"/>
+      <c r="T31" s="15"/>
       <c r="U31" s="15"/>
       <c r="V31" s="15"/>
-      <c r="W31" s="15"/>
+      <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
+      <c r="AA31" s="18"/>
       <c r="AB31" s="18"/>
-      <c r="AC31" s="18"/>
+      <c r="AC31" s="15"/>
       <c r="AD31" s="15"/>
       <c r="AE31" s="15"/>
-      <c r="AF31" s="15"/>
-    </row>
-    <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="9"/>
       <c r="D32" s="12"/>
       <c r="E32" s="14"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
+      <c r="K32" s="16"/>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
+      <c r="N32" s="12"/>
       <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="5"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="18"/>
       <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
+      <c r="T32" s="15"/>
       <c r="U32" s="15"/>
       <c r="V32" s="15"/>
-      <c r="W32" s="15"/>
+      <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
+      <c r="AA32" s="18"/>
       <c r="AB32" s="18"/>
-      <c r="AC32" s="18"/>
+      <c r="AC32" s="15"/>
       <c r="AD32" s="15"/>
       <c r="AE32" s="15"/>
-      <c r="AF32" s="15"/>
-    </row>
-    <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="9"/>
       <c r="D33" s="12"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
+      <c r="K33" s="16"/>
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
+      <c r="N33" s="12"/>
       <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="5"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="18"/>
       <c r="S33" s="18"/>
-      <c r="T33" s="18"/>
+      <c r="T33" s="15"/>
       <c r="U33" s="15"/>
       <c r="V33" s="15"/>
-      <c r="W33" s="15"/>
+      <c r="Y33" s="5"/>
       <c r="Z33" s="5"/>
-      <c r="AA33" s="5"/>
+      <c r="AA33" s="18"/>
       <c r="AB33" s="18"/>
-      <c r="AC33" s="18"/>
+      <c r="AC33" s="15"/>
       <c r="AD33" s="15"/>
       <c r="AE33" s="15"/>
-      <c r="AF33" s="15"/>
-    </row>
-    <row r="34" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="9"/>
       <c r="D34" s="12"/>
       <c r="E34" s="14"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
+      <c r="K34" s="16"/>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
-      <c r="N34" s="16"/>
+      <c r="N34" s="12"/>
       <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="5"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="18"/>
       <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
+      <c r="T34" s="15"/>
       <c r="U34" s="15"/>
       <c r="V34" s="15"/>
-      <c r="W34" s="15"/>
+      <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
-      <c r="AA34" s="5"/>
+      <c r="AA34" s="18"/>
       <c r="AB34" s="18"/>
-      <c r="AC34" s="18"/>
+      <c r="AC34" s="15"/>
       <c r="AD34" s="15"/>
       <c r="AE34" s="15"/>
-      <c r="AF34" s="15"/>
-    </row>
-    <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="9"/>
       <c r="D35" s="12"/>
       <c r="E35" s="14"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
+      <c r="H35" s="12"/>
       <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
+      <c r="K35" s="16"/>
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
-      <c r="N35" s="16"/>
+      <c r="N35" s="12"/>
       <c r="O35" s="12"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="5"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="18"/>
       <c r="S35" s="18"/>
-      <c r="T35" s="18"/>
+      <c r="T35" s="15"/>
       <c r="U35" s="15"/>
       <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
+      <c r="Y35" s="5"/>
       <c r="Z35" s="5"/>
-      <c r="AA35" s="5"/>
+      <c r="AA35" s="18"/>
       <c r="AB35" s="18"/>
-      <c r="AC35" s="18"/>
+      <c r="AC35" s="15"/>
       <c r="AD35" s="15"/>
       <c r="AE35" s="15"/>
-      <c r="AF35" s="15"/>
-    </row>
-    <row r="36" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="9"/>
       <c r="D36" s="12"/>
       <c r="E36" s="14"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
+      <c r="K36" s="16"/>
       <c r="L36" s="16"/>
       <c r="M36" s="16"/>
-      <c r="N36" s="16"/>
+      <c r="N36" s="12"/>
       <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="5"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="18"/>
       <c r="S36" s="18"/>
-      <c r="T36" s="18"/>
+      <c r="T36" s="15"/>
       <c r="U36" s="15"/>
       <c r="V36" s="15"/>
-      <c r="W36" s="15"/>
+      <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
-      <c r="AA36" s="5"/>
+      <c r="AA36" s="18"/>
       <c r="AB36" s="18"/>
-      <c r="AC36" s="18"/>
+      <c r="AC36" s="15"/>
       <c r="AD36" s="15"/>
       <c r="AE36" s="15"/>
-      <c r="AF36" s="15"/>
-    </row>
-    <row r="37" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S37" s="18"/>
-      <c r="AB37" s="18"/>
-    </row>
-    <row r="38" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R37" s="18"/>
+      <c r="AA37" s="18"/>
+    </row>
+    <row r="38" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="12"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="H38" s="15"/>
       <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
+      <c r="K38" s="16"/>
       <c r="L38" s="16"/>
       <c r="M38" s="16"/>
-      <c r="N38" s="16"/>
-      <c r="P38" s="19"/>
-      <c r="R38" s="5"/>
+      <c r="O38" s="19"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="18"/>
       <c r="S38" s="18"/>
-      <c r="T38" s="18"/>
+      <c r="T38" s="15"/>
       <c r="U38" s="15"/>
       <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
+      <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
-      <c r="AA38" s="5"/>
+      <c r="AA38" s="18"/>
       <c r="AB38" s="18"/>
-      <c r="AC38" s="18"/>
+      <c r="AC38" s="15"/>
       <c r="AD38" s="15"/>
       <c r="AE38" s="15"/>
-      <c r="AF38" s="15"/>
-    </row>
-    <row r="39" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="39" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5047,9 +4948,12 @@
     <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="O11:O16"/>
+    <mergeCell ref="R2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5110,9 +5014,9 @@
       <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -5125,34 +5029,34 @@
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="53"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Add Globocan 2020 SA valid data; adjusted KZN valid data
</commit_message>
<xml_diff>
--- a/Config/Reweighted_GlobocanCC_rates.xlsx
+++ b/Config/Reweighted_GlobocanCC_rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B97C17D-52E4-4A8A-B447-72D9D9AF53A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D721F470-CBAD-480F-B754-A11E9558C10A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="387" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CC rates" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
   <si>
     <t>HIV+ RR</t>
   </si>
@@ -186,6 +186,12 @@
   <si>
     <t>Multipliers for broad age groups</t>
   </si>
+  <si>
+    <t>Observed Globocan 2020 CC incidence in SA</t>
+  </si>
+  <si>
+    <t>Multiplier on Globocan 2020 data</t>
+  </si>
 </sst>
 </file>
 
@@ -195,7 +201,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,58 +215,75 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -425,94 +448,116 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -832,7 +877,7 @@
             <c:numRef>
               <c:f>'CC rates'!$AB$4:$AB$15</c:f>
               <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>4.2506211395658813</c:v>
@@ -1223,7 +1268,738 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Adjusted</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Globocan 2018 for KZN</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CC rates'!$B$45:$D$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Observed Globocan 2020 CC incidence in SA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'CC rates'!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>15–19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20–24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25–29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30–34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35–39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40–44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45–49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50–54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55–59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60–64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65-69</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70-74</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CC rates'!$D$47:$D$58</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>81.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>92.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>96.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1548-442E-9FB2-317B44645505}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'CC rates'!$AB$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KZN CC rate (HIV 4x risk) - adjusted older ages</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'CC rates'!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>15–19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20–24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25–29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30–34</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35–39</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40–44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45–49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50–54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55–59</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60–64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65-69</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>70-74</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'CC rates'!$AB$47:$AB$58</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.6201231945624468</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2706329113924051</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.889283653846149</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.364004807692304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.143073789044792</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.961502942507948</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>127.77812147777082</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>144.57450845335003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150.41399999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>151.82413124999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>148.06378124999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>151.66744999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1548-442E-9FB2-317B44645505}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1608309903"/>
+        <c:axId val="1397346463"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1608309903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Age Group</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1397346463"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1397346463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ICC per 100K</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1608309903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.63435889992587902"/>
+          <c:y val="0.66715471988415243"/>
+          <c:w val="0.24223787974805577"/>
+          <c:h val="0.15948411620961173"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1779,6 +2555,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1812,6 +3104,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>1376363</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1B351F1-E355-400B-8246-40D8D3F27550}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2020,8 +3350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE959"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="I40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB47" sqref="AB47:AB58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2034,7 +3364,8 @@
     <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.375" customWidth="1"/>
-    <col min="11" max="14" width="7.625" hidden="1" customWidth="1"/>
+    <col min="11" max="13" width="7.625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="1" customWidth="1"/>
     <col min="15" max="15" width="10.125" customWidth="1"/>
     <col min="16" max="16" width="19.75" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.375" customWidth="1"/>
@@ -2054,7 +3385,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52"/>
+      <c r="A1" s="51"/>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
@@ -2088,12 +3419,12 @@
     </row>
     <row r="2" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="54" t="s">
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="52" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="25"/>
@@ -2110,28 +3441,28 @@
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
-      <c r="P2" s="54" t="s">
+      <c r="P2" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="54" t="s">
+      <c r="Q2" s="52" t="s">
         <v>38</v>
       </c>
       <c r="R2" s="55" t="s">
         <v>44</v>
       </c>
       <c r="S2" s="56"/>
-      <c r="T2" s="53" t="s">
+      <c r="T2" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
       <c r="W2" s="25"/>
       <c r="X2" s="47"/>
       <c r="Y2" s="25"/>
       <c r="Z2" s="25"/>
       <c r="AA2" s="26"/>
     </row>
-    <row r="3" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
@@ -2194,7 +3525,7 @@
       <c r="X3" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" s="58" t="s">
+      <c r="Y3" s="53" t="s">
         <v>50</v>
       </c>
       <c r="Z3" s="42" t="s">
@@ -2234,7 +3565,7 @@
         <v>13.278004340697793</v>
       </c>
       <c r="I4" s="37">
-        <f>D4/(I$1*E4+(1-E4))</f>
+        <f t="shared" ref="I4:I16" si="1">D4/(I$1*E4+(1-E4))</f>
         <v>3.3195010851744482</v>
       </c>
       <c r="J4" s="25"/>
@@ -2247,7 +3578,7 @@
         <v>#REF!</v>
       </c>
       <c r="M4" s="26" t="e">
-        <f t="shared" ref="M4:M16" si="1">SUM(K4+L4)</f>
+        <f t="shared" ref="M4:M16" si="2">SUM(K4+L4)</f>
         <v>#REF!</v>
       </c>
       <c r="N4" s="28" t="e">
@@ -2263,23 +3594,23 @@
         <v>538265</v>
       </c>
       <c r="R4" s="38">
-        <f t="shared" ref="R4:R16" si="2">P4*Q4</f>
+        <f t="shared" ref="R4:R16" si="3">P4*Q4</f>
         <v>50327.777499999997</v>
       </c>
       <c r="S4" s="38">
-        <f t="shared" ref="S4:S16" si="3">Q4-R4</f>
+        <f t="shared" ref="S4:S16" si="4">Q4-R4</f>
         <v>487937.22250000003</v>
       </c>
       <c r="T4" s="41">
-        <f t="shared" ref="T4:T16" si="4">H4*R4/100000</f>
+        <f t="shared" ref="T4:T16" si="5">H4*R4/100000</f>
         <v>6.6825244810267268</v>
       </c>
       <c r="U4" s="41">
-        <f t="shared" ref="U4:U16" si="5">I4*S4/100000</f>
+        <f t="shared" ref="U4:U16" si="6">I4*S4/100000</f>
         <v>16.197081395857563</v>
       </c>
-      <c r="V4" s="41">
-        <f t="shared" ref="V4:V16" si="6">(T4+U4)/Q4*100000</f>
+      <c r="V4" s="37">
+        <f t="shared" ref="V4:V16" si="7">(T4+U4)/Q4*100000</f>
         <v>4.2506211395658813</v>
       </c>
       <c r="W4" s="25"/>
@@ -2287,7 +3618,7 @@
         <v>4</v>
       </c>
       <c r="Y4" s="32">
-        <f>V4/D4</f>
+        <f t="shared" ref="Y4:Y16" si="8">V4/D4</f>
         <v>1.0879354290569245</v>
       </c>
       <c r="Z4" s="32">
@@ -2298,8 +3629,8 @@
         <f>AVERAGE(Y4:Y6)</f>
         <v>1.2195984455181634</v>
       </c>
-      <c r="AB4" s="46">
-        <f>D4*Z4</f>
+      <c r="AB4" s="67">
+        <f t="shared" ref="AB4:AB15" si="9">D4*Z4</f>
         <v>4.2506211395658813</v>
       </c>
       <c r="AC4" s="15"/>
@@ -2314,7 +3645,7 @@
         <v>503</v>
       </c>
       <c r="C5" s="34">
-        <f t="shared" ref="C5:C15" si="7">B5/(D5/100000)</f>
+        <f t="shared" ref="C5:C15" si="10">B5/(D5/100000)</f>
         <v>2550891.9999999995</v>
       </c>
       <c r="D5" s="35">
@@ -2330,7 +3661,7 @@
         <v>52.547881559160174</v>
       </c>
       <c r="I5" s="37">
-        <f>D5/(I$1*E5+(1-E5))</f>
+        <f t="shared" si="1"/>
         <v>13.136970389790044</v>
       </c>
       <c r="J5" s="25"/>
@@ -2343,7 +3674,7 @@
         <v>#REF!</v>
       </c>
       <c r="M5" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N5" s="28" t="e">
@@ -2359,23 +3690,23 @@
         <v>543645</v>
       </c>
       <c r="R5" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>181686.15899999999</v>
       </c>
       <c r="S5" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>361958.84100000001</v>
       </c>
       <c r="T5" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>95.472227640707416</v>
       </c>
       <c r="U5" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>47.550425765397222</v>
       </c>
-      <c r="V5" s="41">
-        <f t="shared" si="6"/>
+      <c r="V5" s="37">
+        <f t="shared" si="7"/>
         <v>26.30809690259354</v>
       </c>
       <c r="W5" s="25"/>
@@ -2384,16 +3715,16 @@
         <v>5</v>
       </c>
       <c r="Y5" s="32">
-        <f>V5/D5</f>
+        <f t="shared" si="8"/>
         <v>1.3341772151898736</v>
       </c>
       <c r="Z5" s="32">
-        <f t="shared" ref="Z5:Z13" si="8">Y5</f>
+        <f t="shared" ref="Z5:Z13" si="11">Y5</f>
         <v>1.3341772151898736</v>
       </c>
       <c r="AA5" s="45"/>
-      <c r="AB5" s="46">
-        <f>D5*Z5</f>
+      <c r="AB5" s="67">
+        <f t="shared" si="9"/>
         <v>26.308096902593544</v>
       </c>
       <c r="AC5" s="15"/>
@@ -2408,7 +3739,7 @@
         <v>913</v>
       </c>
       <c r="C6" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2549183</v>
       </c>
       <c r="D6" s="35">
@@ -2426,7 +3757,7 @@
         <v>68.875762578411624</v>
       </c>
       <c r="I6" s="37">
-        <f>D6/(I$1*E6+(1-E6))</f>
+        <f t="shared" si="1"/>
         <v>17.218940644602906</v>
       </c>
       <c r="J6" s="25"/>
@@ -2439,7 +3770,7 @@
         <v>#REF!</v>
       </c>
       <c r="M6" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N6" s="28" t="e">
@@ -2455,23 +3786,23 @@
         <v>529822</v>
       </c>
       <c r="R6" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>277679.71020000003</v>
       </c>
       <c r="S6" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>252142.28979999997</v>
       </c>
       <c r="T6" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>191.25401792577344</v>
       </c>
       <c r="U6" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43.416231220604637</v>
       </c>
-      <c r="V6" s="41">
-        <f t="shared" si="6"/>
+      <c r="V6" s="37">
+        <f t="shared" si="7"/>
         <v>44.29228102011205</v>
       </c>
       <c r="W6" s="25"/>
@@ -2480,16 +3811,16 @@
         <v>6</v>
       </c>
       <c r="Y6" s="32">
-        <f>V6/D6</f>
-        <v>1.2366826923076921</v>
-      </c>
-      <c r="Z6" s="32">
         <f t="shared" si="8"/>
         <v>1.2366826923076921</v>
       </c>
+      <c r="Z6" s="32">
+        <f t="shared" si="11"/>
+        <v>1.2366826923076921</v>
+      </c>
       <c r="AA6" s="45"/>
-      <c r="AB6" s="46">
-        <f>D6*Z6</f>
+      <c r="AB6" s="67">
+        <f t="shared" si="9"/>
         <v>44.29228102011205</v>
       </c>
       <c r="AC6" s="15"/>
@@ -2504,7 +3835,7 @@
         <v>1310</v>
       </c>
       <c r="C7" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2437030</v>
       </c>
       <c r="D7" s="35">
@@ -2520,7 +3851,7 @@
         <v>103.37298963208369</v>
       </c>
       <c r="I7" s="37">
-        <f>D7/(I$1*E7+(1-E7))</f>
+        <f t="shared" si="1"/>
         <v>25.843247408020922</v>
       </c>
       <c r="J7" s="25"/>
@@ -2533,7 +3864,7 @@
         <v>#REF!</v>
       </c>
       <c r="M7" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N7" s="28" t="e">
@@ -2549,44 +3880,44 @@
         <v>446915</v>
       </c>
       <c r="R7" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>281958.67350000003</v>
       </c>
       <c r="S7" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>164956.32649999997</v>
       </c>
       <c r="T7" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>291.46911032391574</v>
       </c>
       <c r="U7" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42.630071572577769</v>
       </c>
-      <c r="V7" s="41">
-        <f t="shared" si="6"/>
+      <c r="V7" s="37">
+        <f t="shared" si="7"/>
         <v>74.756761777182135</v>
       </c>
       <c r="W7" s="25"/>
       <c r="X7" s="38">
-        <f t="shared" ref="X7:X16" si="9">X6+1</f>
+        <f t="shared" ref="X7:X16" si="12">X6+1</f>
         <v>7</v>
       </c>
       <c r="Y7" s="32">
-        <f>V7/D7</f>
+        <f t="shared" si="8"/>
         <v>1.3907211538461539</v>
       </c>
       <c r="Z7" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.3907211538461539</v>
       </c>
       <c r="AA7" s="45">
         <f>AVERAGE(Y7:Y10)</f>
         <v>1.4018326814868265</v>
       </c>
-      <c r="AB7" s="46">
-        <f>D7*Z7</f>
+      <c r="AB7" s="67">
+        <f t="shared" si="9"/>
         <v>74.756761777182135</v>
       </c>
       <c r="AC7" s="15"/>
@@ -2601,7 +3932,7 @@
         <v>1501</v>
       </c>
       <c r="C8" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2108701</v>
       </c>
       <c r="D8" s="35">
@@ -2619,7 +3950,7 @@
         <v>128.89318746476422</v>
       </c>
       <c r="I8" s="37">
-        <f>D8/(I$1*E8+(1-E8))</f>
+        <f t="shared" si="1"/>
         <v>32.223296866191056</v>
       </c>
       <c r="J8" s="25"/>
@@ -2632,7 +3963,7 @@
         <v>#REF!</v>
       </c>
       <c r="M8" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N8" s="28" t="e">
@@ -2648,41 +3979,41 @@
         <v>348503</v>
       </c>
       <c r="R8" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>233322.7585</v>
       </c>
       <c r="S8" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>115180.2415</v>
       </c>
       <c r="T8" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>300.73714051136409</v>
       </c>
       <c r="U8" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37.114871149740793</v>
       </c>
-      <c r="V8" s="41">
-        <f t="shared" si="6"/>
+      <c r="V8" s="37">
+        <f t="shared" si="7"/>
         <v>96.943788621935781</v>
       </c>
       <c r="W8" s="25"/>
       <c r="X8" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="Y8" s="32">
-        <f>V8/D8</f>
-        <v>1.3619284744228155</v>
-      </c>
-      <c r="Z8" s="32">
         <f t="shared" si="8"/>
         <v>1.3619284744228155</v>
       </c>
+      <c r="Z8" s="32">
+        <f t="shared" si="11"/>
+        <v>1.3619284744228155</v>
+      </c>
       <c r="AA8" s="45"/>
-      <c r="AB8" s="46">
-        <f>D8*Z8</f>
+      <c r="AB8" s="67">
+        <f t="shared" si="9"/>
         <v>96.943788621935781</v>
       </c>
       <c r="AC8" s="15"/>
@@ -2697,7 +4028,7 @@
         <v>1511</v>
       </c>
       <c r="C9" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1775756</v>
       </c>
       <c r="D9" s="35">
@@ -2713,7 +4044,7 @@
         <v>154.07970881476177</v>
       </c>
       <c r="I9" s="37">
-        <f>D9/(I$1*E9+(1-E9))</f>
+        <f t="shared" si="1"/>
         <v>38.519927203690443</v>
       </c>
       <c r="J9" s="25"/>
@@ -2726,7 +4057,7 @@
         <v>#REF!</v>
       </c>
       <c r="M9" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N9" s="28" t="e">
@@ -2742,41 +4073,41 @@
         <v>282350</v>
       </c>
       <c r="R9" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>173024.08000000002</v>
       </c>
       <c r="S9" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>109325.91999999998</v>
       </c>
       <c r="T9" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>266.59499864342047</v>
       </c>
       <c r="U9" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42.112264798764848</v>
       </c>
-      <c r="V9" s="41">
-        <f t="shared" si="6"/>
+      <c r="V9" s="37">
+        <f t="shared" si="7"/>
         <v>109.33496137495494</v>
       </c>
       <c r="W9" s="25"/>
       <c r="X9" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="Y9" s="32">
-        <f>V9/D9</f>
-        <v>1.2849253055681302</v>
-      </c>
-      <c r="Z9" s="32">
         <f t="shared" si="8"/>
         <v>1.2849253055681302</v>
       </c>
+      <c r="Z9" s="32">
+        <f t="shared" si="11"/>
+        <v>1.2849253055681302</v>
+      </c>
       <c r="AA9" s="45"/>
-      <c r="AB9" s="46">
-        <f>D9*Z9</f>
+      <c r="AB9" s="67">
+        <f t="shared" si="9"/>
         <v>109.33496137495494</v>
       </c>
       <c r="AC9" s="15"/>
@@ -2791,7 +4122,7 @@
         <v>1498</v>
       </c>
       <c r="C10" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1569513</v>
       </c>
       <c r="D10" s="35">
@@ -2809,7 +4140,7 @@
         <v>239.05727864301082</v>
       </c>
       <c r="I10" s="37">
-        <f>D10/(I$1*E10+(1-E10))</f>
+        <f t="shared" si="1"/>
         <v>59.764319660752705</v>
       </c>
       <c r="J10" s="25"/>
@@ -2822,7 +4153,7 @@
         <v>#REF!</v>
       </c>
       <c r="M10" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N10" s="28" t="e">
@@ -2838,41 +4169,41 @@
         <v>243989</v>
       </c>
       <c r="R10" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>122555.67469999999</v>
       </c>
       <c r="S10" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>121433.32530000001</v>
       </c>
       <c r="T10" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>292.97826076040087</v>
       </c>
       <c r="U10" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72.573800706973685</v>
       </c>
-      <c r="V10" s="41">
-        <f t="shared" si="6"/>
+      <c r="V10" s="37">
+        <f t="shared" si="7"/>
         <v>149.82317295754092</v>
       </c>
       <c r="W10" s="25"/>
       <c r="X10" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="Y10" s="32">
-        <f>V10/D10</f>
-        <v>1.5697557921102063</v>
-      </c>
-      <c r="Z10" s="32">
         <f t="shared" si="8"/>
         <v>1.5697557921102063</v>
       </c>
+      <c r="Z10" s="32">
+        <f t="shared" si="11"/>
+        <v>1.5697557921102063</v>
+      </c>
       <c r="AA10" s="45"/>
-      <c r="AB10" s="46">
-        <f>D10*Z10</f>
+      <c r="AB10" s="67">
+        <f t="shared" si="9"/>
         <v>149.82317295754092</v>
       </c>
       <c r="AC10" s="15"/>
@@ -2887,7 +4218,7 @@
         <v>1320</v>
       </c>
       <c r="C11" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1373576.0000000002</v>
       </c>
       <c r="D11" s="35">
@@ -2903,7 +4234,7 @@
         <v>240.70012313525373</v>
       </c>
       <c r="I11" s="37">
-        <f>D11/(I$1*E11+(1-E11))</f>
+        <f t="shared" si="1"/>
         <v>60.175030783813433</v>
       </c>
       <c r="J11" s="25"/>
@@ -2916,7 +4247,7 @@
         <v>#REF!</v>
       </c>
       <c r="M11" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N11" s="28" t="e">
@@ -2927,51 +4258,51 @@
         <v>37</v>
       </c>
       <c r="P11" s="39">
-        <f t="shared" ref="P11:P16" si="10">0.5023</f>
+        <f t="shared" ref="P11:P16" si="13">0.5023</f>
         <v>0.50229999999999997</v>
       </c>
       <c r="Q11" s="40">
         <v>216352</v>
       </c>
       <c r="R11" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>108673.6096</v>
       </c>
       <c r="S11" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>107678.3904</v>
       </c>
       <c r="T11" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>261.5775121227249</v>
       </c>
       <c r="U11" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>64.795504570714812</v>
       </c>
-      <c r="V11" s="41">
-        <f t="shared" si="6"/>
+      <c r="V11" s="37">
+        <f t="shared" si="7"/>
         <v>150.85278467194186</v>
       </c>
       <c r="W11" s="25"/>
       <c r="X11" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="Y11" s="32">
-        <f>V11/D11</f>
+        <f t="shared" si="8"/>
         <v>1.5697557921102063</v>
       </c>
       <c r="Z11" s="32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1.5697557921102063</v>
       </c>
       <c r="AA11" s="45">
         <f>AVERAGE(Y11:Y13)</f>
         <v>1.5677935973700687</v>
       </c>
-      <c r="AB11" s="46">
-        <f>D11*Z11</f>
+      <c r="AB11" s="67">
+        <f t="shared" si="9"/>
         <v>150.85278467194186</v>
       </c>
       <c r="AC11" s="15"/>
@@ -2986,7 +4317,7 @@
         <v>1123</v>
       </c>
       <c r="C12" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1183955</v>
       </c>
       <c r="D12" s="35">
@@ -3004,7 +4335,7 @@
         <v>237.12894493456253</v>
       </c>
       <c r="I12" s="37">
-        <f>D12/(I$1*E12+(1-E12))</f>
+        <f t="shared" si="1"/>
         <v>59.282236233640631</v>
       </c>
       <c r="J12" s="25"/>
@@ -3017,7 +4348,7 @@
         <v>#REF!</v>
       </c>
       <c r="M12" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N12" s="28" t="e">
@@ -3026,48 +4357,48 @@
       </c>
       <c r="O12" s="57"/>
       <c r="P12" s="39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
       </c>
       <c r="Q12" s="40">
         <v>189489</v>
       </c>
       <c r="R12" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95180.324699999997</v>
       </c>
       <c r="S12" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>94308.675300000003</v>
       </c>
       <c r="T12" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>225.70009974640084</v>
       </c>
       <c r="U12" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>55.908291680163096</v>
       </c>
-      <c r="V12" s="41">
-        <f t="shared" si="6"/>
+      <c r="V12" s="37">
+        <f t="shared" si="7"/>
         <v>148.61463801411369</v>
       </c>
       <c r="W12" s="25"/>
       <c r="X12" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="Y12" s="32">
-        <f>V12/D12</f>
-        <v>1.5668124999999999</v>
-      </c>
-      <c r="Z12" s="32">
         <f t="shared" si="8"/>
         <v>1.5668124999999999</v>
       </c>
+      <c r="Z12" s="32">
+        <f t="shared" si="11"/>
+        <v>1.5668124999999999</v>
+      </c>
       <c r="AA12" s="45"/>
-      <c r="AB12" s="46">
-        <f>D12*Z12</f>
+      <c r="AB12" s="67">
+        <f t="shared" si="9"/>
         <v>148.61463801411369</v>
       </c>
       <c r="AC12" s="15"/>
@@ -3082,7 +4413,7 @@
         <v>966</v>
       </c>
       <c r="C13" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>990896</v>
       </c>
       <c r="D13" s="35">
@@ -3098,7 +4429,7 @@
         <v>243.71881610179068</v>
       </c>
       <c r="I13" s="37">
-        <f>D13/(I$1*E13+(1-E13))</f>
+        <f t="shared" si="1"/>
         <v>60.92970402544767</v>
       </c>
       <c r="J13" s="25"/>
@@ -3111,7 +4442,7 @@
         <v>#REF!</v>
       </c>
       <c r="M13" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N13" s="28" t="e">
@@ -3120,48 +4451,48 @@
       </c>
       <c r="O13" s="57"/>
       <c r="P13" s="39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
       </c>
       <c r="Q13" s="40">
         <v>163816</v>
       </c>
       <c r="R13" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82284.776799999992</v>
       </c>
       <c r="S13" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>81531.223200000008</v>
       </c>
       <c r="T13" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>200.54348384896093</v>
       </c>
       <c r="U13" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>49.676732984087131</v>
       </c>
-      <c r="V13" s="41">
-        <f t="shared" si="6"/>
+      <c r="V13" s="37">
+        <f t="shared" si="7"/>
         <v>152.74467502139476</v>
       </c>
       <c r="W13" s="25"/>
       <c r="X13" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="Y13" s="32">
-        <f>V13/D13</f>
-        <v>1.5668124999999997</v>
-      </c>
-      <c r="Z13" s="32">
         <f t="shared" si="8"/>
         <v>1.5668124999999997</v>
       </c>
+      <c r="Z13" s="32">
+        <f t="shared" si="11"/>
+        <v>1.5668124999999997</v>
+      </c>
       <c r="AA13" s="45"/>
-      <c r="AB13" s="46">
-        <f>D13*Z13</f>
+      <c r="AB13" s="67">
+        <f t="shared" si="9"/>
         <v>152.74467502139476</v>
       </c>
       <c r="AC13" s="15"/>
@@ -3176,7 +4507,7 @@
         <v>766</v>
       </c>
       <c r="C14" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>751066.99999999988</v>
       </c>
       <c r="D14" s="35">
@@ -3194,7 +4525,7 @@
         <v>351.98701662344729</v>
       </c>
       <c r="I14" s="37">
-        <f>D14/(I$1*E14+(1-E14))</f>
+        <f t="shared" si="1"/>
         <v>87.996754155861822</v>
       </c>
       <c r="J14" s="25"/>
@@ -3207,7 +4538,7 @@
         <v>#REF!</v>
       </c>
       <c r="M14" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N14" s="28" t="e">
@@ -3216,39 +4547,39 @@
       </c>
       <c r="O14" s="57"/>
       <c r="P14" s="39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
       </c>
       <c r="Q14" s="40">
         <v>134732</v>
       </c>
       <c r="R14" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67675.883600000001</v>
       </c>
       <c r="S14" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67056.116399999999</v>
       </c>
       <c r="T14" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>238.21032365719682</v>
       </c>
       <c r="U14" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>59.007205894976536</v>
       </c>
-      <c r="V14" s="41">
-        <f t="shared" si="6"/>
+      <c r="V14" s="37">
+        <f t="shared" si="7"/>
         <v>220.59906299332997</v>
       </c>
       <c r="W14" s="25"/>
       <c r="X14" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="Y14" s="32">
-        <f>V14/D14</f>
+        <f t="shared" si="8"/>
         <v>2.1629853321829158</v>
       </c>
       <c r="Z14" s="32">
@@ -3256,8 +4587,8 @@
         <v>1.5668124999999997</v>
       </c>
       <c r="AA14" s="45"/>
-      <c r="AB14" s="46">
-        <f>D14*Z14</f>
+      <c r="AB14" s="67">
+        <f t="shared" si="9"/>
         <v>159.7964462557934</v>
       </c>
       <c r="AC14" s="15"/>
@@ -3272,7 +4603,7 @@
         <v>562</v>
       </c>
       <c r="C15" s="34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>508942</v>
       </c>
       <c r="D15" s="35">
@@ -3288,7 +4619,7 @@
         <v>381.10494046983166</v>
       </c>
       <c r="I15" s="37">
-        <f>D15/(I$1*E15+(1-E15))</f>
+        <f t="shared" si="1"/>
         <v>95.276235117457915</v>
       </c>
       <c r="J15" s="25"/>
@@ -3301,7 +4632,7 @@
         <v>#REF!</v>
       </c>
       <c r="M15" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
       <c r="N15" s="28" t="e">
@@ -3310,48 +4641,48 @@
       </c>
       <c r="O15" s="57"/>
       <c r="P15" s="39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
       </c>
       <c r="Q15" s="40">
         <v>93602</v>
       </c>
       <c r="R15" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47016.284599999999</v>
       </c>
       <c r="S15" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46585.715400000001</v>
       </c>
       <c r="T15" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>179.1813834359566</v>
       </c>
       <c r="U15" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44.385115735653798</v>
       </c>
-      <c r="V15" s="41">
-        <f t="shared" si="6"/>
+      <c r="V15" s="37">
+        <f t="shared" si="7"/>
         <v>238.84799381595525</v>
       </c>
       <c r="W15" s="25"/>
       <c r="X15" s="38">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="Y15" s="32">
+        <f t="shared" si="8"/>
+        <v>2.1629853321829162</v>
+      </c>
+      <c r="Z15" s="32">
+        <f t="shared" ref="Z15" si="14">Z14</f>
+        <v>1.5668124999999997</v>
+      </c>
+      <c r="AA15" s="45"/>
+      <c r="AB15" s="67">
         <f t="shared" si="9"/>
-        <v>15</v>
-      </c>
-      <c r="Y15" s="32">
-        <f>V15/D15</f>
-        <v>2.1629853321829162</v>
-      </c>
-      <c r="Z15" s="32">
-        <f t="shared" ref="Z15" si="11">Z14</f>
-        <v>1.5668124999999997</v>
-      </c>
-      <c r="AA15" s="45"/>
-      <c r="AB15" s="46">
-        <f>D15*Z15</f>
         <v>173.01551552043256</v>
       </c>
       <c r="AC15" s="15"/>
@@ -3381,7 +4712,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="I16" s="37" t="e">
-        <f>D16/(I$1*E16+(1-E16))</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="J16" s="25"/>
@@ -3394,7 +4725,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="M16" s="26" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="N16" s="28" t="e">
@@ -3403,39 +4734,39 @@
       </c>
       <c r="O16" s="57"/>
       <c r="P16" s="39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
       </c>
       <c r="Q16" s="40">
         <v>58431</v>
       </c>
       <c r="R16" s="38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29349.891299999999</v>
       </c>
       <c r="S16" s="38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29081.108700000001</v>
       </c>
       <c r="T16" s="41" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U16" s="41" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="V16" s="41" t="e">
+      <c r="U16" s="41" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
+      <c r="V16" s="41" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="W16" s="25"/>
       <c r="X16" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
       <c r="Y16" s="32" t="e">
-        <f>V16/D16</f>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z16" s="32"/>
@@ -3479,11 +4810,11 @@
         <v>18</v>
       </c>
       <c r="B18" s="27">
-        <f t="shared" ref="B18:C18" si="12">SUM(B4:B16)</f>
+        <f t="shared" ref="B18:C18" si="15">SUM(B4:B16)</f>
         <v>12975</v>
       </c>
       <c r="C18" s="27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>20358985</v>
       </c>
       <c r="D18" s="28">
@@ -3503,11 +4834,11 @@
       </c>
       <c r="J18" s="25"/>
       <c r="K18" s="26" t="e">
-        <f t="shared" ref="K18:L18" si="13">SUM(K4:K16)</f>
+        <f t="shared" ref="K18:L18" si="16">SUM(K4:K16)</f>
         <v>#REF!</v>
       </c>
       <c r="L18" s="26" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>#REF!</v>
       </c>
       <c r="M18" s="26"/>
@@ -3515,23 +4846,23 @@
       <c r="O18" s="30"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="27">
-        <f t="shared" ref="Q18:U18" si="14">SUM(Q4:Q16)</f>
+        <f t="shared" ref="Q18:U18" si="17">SUM(Q4:Q16)</f>
         <v>3789911</v>
       </c>
       <c r="R18" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>1750735.6040000003</v>
       </c>
       <c r="S18" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>2039175.3959999997</v>
       </c>
       <c r="T18" s="29" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="U18" s="29" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
       <c r="V18" s="29" t="e">
@@ -4031,27 +5362,1462 @@
     <row r="41" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="51"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="I44" s="36">
+        <v>4</v>
+      </c>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="25"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="25"/>
+      <c r="T44" s="25"/>
+      <c r="U44" s="25"/>
+      <c r="V44" s="25"/>
+      <c r="W44" s="25"/>
+      <c r="X44" s="25"/>
+      <c r="Y44" s="25"/>
+      <c r="Z44" s="25"/>
+      <c r="AA44" s="26"/>
+      <c r="AB44" s="50"/>
+    </row>
+    <row r="45" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="31"/>
+      <c r="B45" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="I45" s="56"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L45" s="25"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="25"/>
+      <c r="P45" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q45" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="R45" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="S45" s="56"/>
+      <c r="T45" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="U45" s="54"/>
+      <c r="V45" s="54"/>
+      <c r="W45" s="25"/>
+      <c r="X45" s="47"/>
+      <c r="Y45" s="25"/>
+      <c r="Z45" s="25"/>
+      <c r="AA45" s="26"/>
+      <c r="AB45" s="50"/>
+    </row>
+    <row r="46" spans="1:31" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="J46" s="25"/>
+      <c r="K46" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="L46" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="M46" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="N46" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="O46" s="27"/>
+      <c r="P46" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q46" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="R46" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="S46" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="T46" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="U46" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="V46" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="W46" s="25"/>
+      <c r="X46" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y46" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z46" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA46" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB46" s="44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="62">
+        <v>14</v>
+      </c>
+      <c r="C47" s="61">
+        <f>B47/(D47/100000)</f>
+        <v>2456140.3508771933</v>
+      </c>
+      <c r="D47" s="63">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E47" s="32">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="37">
+        <f>I$44*I47</f>
+        <v>1.9371282922684789</v>
+      </c>
+      <c r="I47" s="37">
+        <f>D47/(I$44*E47+(1-E47))</f>
+        <v>0.48428207306711973</v>
+      </c>
+      <c r="J47" s="25"/>
+      <c r="K47" s="26" t="e">
+        <f>H47*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L47" s="26" t="e">
+        <f>I47*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M47" s="26" t="e">
+        <f t="shared" ref="M47:M59" si="18">SUM(K47+L47)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N47" s="28" t="e">
+        <f>(H47*(#REF!/C47))+(I47*(#REF!/C47))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O47" s="28"/>
+      <c r="P47" s="39">
+        <f>0.0935</f>
+        <v>9.35E-2</v>
+      </c>
+      <c r="Q47" s="40">
+        <v>538265</v>
+      </c>
+      <c r="R47" s="38">
+        <f t="shared" ref="R47:R59" si="19">P47*Q47</f>
+        <v>50327.777499999997</v>
+      </c>
+      <c r="S47" s="38">
+        <f t="shared" ref="S47:S59" si="20">Q47-R47</f>
+        <v>487937.22250000003</v>
+      </c>
+      <c r="T47" s="41">
+        <f t="shared" ref="T47:T59" si="21">H47*R47/100000</f>
+        <v>0.97491361682242972</v>
+      </c>
+      <c r="U47" s="41">
+        <f t="shared" ref="U47:U59" si="22">I47*S47/100000</f>
+        <v>2.3629924963891247</v>
+      </c>
+      <c r="V47" s="66">
+        <f t="shared" ref="V47:V59" si="23">(T47+U47)/Q47*100000</f>
+        <v>0.6201231945624468</v>
+      </c>
+      <c r="W47" s="25"/>
+      <c r="X47" s="48">
+        <v>4</v>
+      </c>
+      <c r="Y47" s="32">
+        <f t="shared" ref="Y47:Y59" si="24">V47/D47</f>
+        <v>1.0879354290569243</v>
+      </c>
+      <c r="Z47" s="32">
+        <f>Y47</f>
+        <v>1.0879354290569243</v>
+      </c>
+      <c r="AA47" s="45">
+        <f>AVERAGE(Y47:Y49)</f>
+        <v>1.2195984455181632</v>
+      </c>
+      <c r="AB47" s="46">
+        <f t="shared" ref="AB47:AB58" si="25">D47*Z47</f>
+        <v>0.6201231945624468</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="62">
+        <v>114</v>
+      </c>
+      <c r="C48" s="61">
+        <f t="shared" ref="C48:C58" si="26">B48/(D48/100000)</f>
+        <v>2425531.9148936169</v>
+      </c>
+      <c r="D48" s="63">
+        <v>4.7</v>
+      </c>
+      <c r="E48" s="32">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="37">
+        <f t="shared" ref="H48:H58" si="27">I$44*I48</f>
+        <v>12.524983344437043</v>
+      </c>
+      <c r="I48" s="37">
+        <f t="shared" ref="I48:I58" si="28">D48/(I$44*E48+(1-E48))</f>
+        <v>3.1312458361092608</v>
+      </c>
+      <c r="J48" s="25"/>
+      <c r="K48" s="26" t="e">
+        <f>H48*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L48" s="26" t="e">
+        <f>I48*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M48" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N48" s="28" t="e">
+        <f>(H48*(#REF!/C48))+(I48*(#REF!/C48))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O48" s="28"/>
+      <c r="P48" s="39">
+        <f>0.3342</f>
+        <v>0.3342</v>
+      </c>
+      <c r="Q48" s="40">
+        <v>543645</v>
+      </c>
+      <c r="R48" s="38">
+        <f t="shared" si="19"/>
+        <v>181686.15899999999</v>
+      </c>
+      <c r="S48" s="38">
+        <f t="shared" si="20"/>
+        <v>361958.84100000001</v>
+      </c>
+      <c r="T48" s="41">
+        <f t="shared" si="21"/>
+        <v>22.756161153897402</v>
+      </c>
+      <c r="U48" s="41">
+        <f t="shared" si="22"/>
+        <v>11.33382113724184</v>
+      </c>
+      <c r="V48" s="66">
+        <f t="shared" si="23"/>
+        <v>6.2706329113924051</v>
+      </c>
+      <c r="W48" s="25"/>
+      <c r="X48" s="38">
+        <f>X47+1</f>
+        <v>5</v>
+      </c>
+      <c r="Y48" s="32">
+        <f t="shared" si="24"/>
+        <v>1.3341772151898734</v>
+      </c>
+      <c r="Z48" s="32">
+        <f t="shared" ref="Z48:Z56" si="29">Y48</f>
+        <v>1.3341772151898734</v>
+      </c>
+      <c r="AA48" s="45"/>
+      <c r="AB48" s="46">
+        <f t="shared" si="25"/>
+        <v>6.2706329113924051</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" s="62">
+        <v>459</v>
+      </c>
+      <c r="C49" s="61">
+        <f t="shared" si="26"/>
+        <v>2593220.338983051</v>
+      </c>
+      <c r="D49" s="63">
+        <v>17.7</v>
+      </c>
+      <c r="E49" s="32">
+        <v>0.36</v>
+      </c>
+      <c r="F49" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" s="25"/>
+      <c r="H49" s="37">
+        <f t="shared" si="27"/>
+        <v>34.038461538461533</v>
+      </c>
+      <c r="I49" s="37">
+        <f t="shared" si="28"/>
+        <v>8.5096153846153832</v>
+      </c>
+      <c r="J49" s="25"/>
+      <c r="K49" s="26" t="e">
+        <f>H49*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L49" s="26" t="e">
+        <f>I49*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M49" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N49" s="28" t="e">
+        <f>(H49*(#REF!/C49))+(I49*(#REF!/C49))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O49" s="28"/>
+      <c r="P49" s="39">
+        <f>0.5241</f>
+        <v>0.52410000000000001</v>
+      </c>
+      <c r="Q49" s="40">
+        <v>529822</v>
+      </c>
+      <c r="R49" s="38">
+        <f t="shared" si="19"/>
+        <v>277679.71020000003</v>
+      </c>
+      <c r="S49" s="38">
+        <f t="shared" si="20"/>
+        <v>252142.28979999997</v>
+      </c>
+      <c r="T49" s="41">
+        <f t="shared" si="21"/>
+        <v>94.517901356538459</v>
+      </c>
+      <c r="U49" s="41">
+        <f t="shared" si="22"/>
+        <v>21.4563390839423</v>
+      </c>
+      <c r="V49" s="66">
+        <f t="shared" si="23"/>
+        <v>21.889283653846149</v>
+      </c>
+      <c r="W49" s="25"/>
+      <c r="X49" s="38">
+        <f>X48+1</f>
+        <v>6</v>
+      </c>
+      <c r="Y49" s="32">
+        <f t="shared" si="24"/>
+        <v>1.2366826923076921</v>
+      </c>
+      <c r="Z49" s="32">
+        <f t="shared" si="29"/>
+        <v>1.2366826923076921</v>
+      </c>
+      <c r="AA49" s="45"/>
+      <c r="AB49" s="46">
+        <f t="shared" si="25"/>
+        <v>21.889283653846149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="62">
+        <v>851</v>
+      </c>
+      <c r="C50" s="61">
+        <f t="shared" si="26"/>
+        <v>2667711.5987460813</v>
+      </c>
+      <c r="D50" s="63">
+        <v>31.9</v>
+      </c>
+      <c r="E50" s="32">
+        <v>0.36</v>
+      </c>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="37">
+        <f t="shared" si="27"/>
+        <v>61.34615384615384</v>
+      </c>
+      <c r="I50" s="37">
+        <f t="shared" si="28"/>
+        <v>15.33653846153846</v>
+      </c>
+      <c r="J50" s="25"/>
+      <c r="K50" s="26" t="e">
+        <f>H50*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L50" s="26" t="e">
+        <f>I50*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M50" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N50" s="28" t="e">
+        <f>(H50*(#REF!/C50))+(I50*(#REF!/C50))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O50" s="28"/>
+      <c r="P50" s="39">
+        <f>0.6309</f>
+        <v>0.63090000000000002</v>
+      </c>
+      <c r="Q50" s="40">
+        <v>446915</v>
+      </c>
+      <c r="R50" s="38">
+        <f t="shared" si="19"/>
+        <v>281958.67350000003</v>
+      </c>
+      <c r="S50" s="38">
+        <f t="shared" si="20"/>
+        <v>164956.32649999997</v>
+      </c>
+      <c r="T50" s="41">
+        <f t="shared" si="21"/>
+        <v>172.97080162788461</v>
+      </c>
+      <c r="U50" s="41">
+        <f t="shared" si="22"/>
+        <v>25.298590458413457</v>
+      </c>
+      <c r="V50" s="66">
+        <f t="shared" si="23"/>
+        <v>44.364004807692304</v>
+      </c>
+      <c r="W50" s="25"/>
+      <c r="X50" s="38">
+        <f t="shared" ref="X50:X59" si="30">X49+1</f>
+        <v>7</v>
+      </c>
+      <c r="Y50" s="32">
+        <f t="shared" si="24"/>
+        <v>1.3907211538461537</v>
+      </c>
+      <c r="Z50" s="32">
+        <f t="shared" si="29"/>
+        <v>1.3907211538461537</v>
+      </c>
+      <c r="AA50" s="45">
+        <f>AVERAGE(Y50:Y53)</f>
+        <v>1.4018326814868265</v>
+      </c>
+      <c r="AB50" s="46">
+        <f t="shared" si="25"/>
+        <v>44.364004807692304</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="62">
+        <v>1171</v>
+      </c>
+      <c r="C51" s="61">
+        <f t="shared" si="26"/>
+        <v>2375253.5496957405</v>
+      </c>
+      <c r="D51" s="63">
+        <v>49.3</v>
+      </c>
+      <c r="E51" s="32">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="F51" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" s="25"/>
+      <c r="H51" s="37">
+        <f t="shared" si="27"/>
+        <v>89.271163422363045</v>
+      </c>
+      <c r="I51" s="37">
+        <f t="shared" si="28"/>
+        <v>22.317790855590761</v>
+      </c>
+      <c r="J51" s="25"/>
+      <c r="K51" s="26" t="e">
+        <f>H51*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L51" s="26" t="e">
+        <f>I51*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M51" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N51" s="28" t="e">
+        <f>(H51*(#REF!/C51))+(I51*(#REF!/C51))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O51" s="28"/>
+      <c r="P51" s="39">
+        <f>0.6695</f>
+        <v>0.66949999999999998</v>
+      </c>
+      <c r="Q51" s="40">
+        <v>348503</v>
+      </c>
+      <c r="R51" s="38">
+        <f t="shared" si="19"/>
+        <v>233322.7585</v>
+      </c>
+      <c r="S51" s="38">
+        <f t="shared" si="20"/>
+        <v>115180.2415</v>
+      </c>
+      <c r="T51" s="41">
+        <f t="shared" si="21"/>
+        <v>208.28994104210045</v>
+      </c>
+      <c r="U51" s="41">
+        <f t="shared" si="22"/>
+        <v>25.705685404934357</v>
+      </c>
+      <c r="V51" s="66">
+        <f t="shared" si="23"/>
+        <v>67.143073789044792</v>
+      </c>
+      <c r="W51" s="25"/>
+      <c r="X51" s="38">
+        <f t="shared" si="30"/>
+        <v>8</v>
+      </c>
+      <c r="Y51" s="32">
+        <f t="shared" si="24"/>
+        <v>1.3619284744228153</v>
+      </c>
+      <c r="Z51" s="32">
+        <f t="shared" si="29"/>
+        <v>1.3619284744228153</v>
+      </c>
+      <c r="AA51" s="45"/>
+      <c r="AB51" s="46">
+        <f t="shared" si="25"/>
+        <v>67.143073789044792</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="62">
+        <v>1283</v>
+      </c>
+      <c r="C52" s="61">
+        <f t="shared" si="26"/>
+        <v>1917787.7428998502</v>
+      </c>
+      <c r="D52" s="63">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="E52" s="32">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="37">
+        <f t="shared" si="27"/>
+        <v>121.14078768673609</v>
+      </c>
+      <c r="I52" s="37">
+        <f t="shared" si="28"/>
+        <v>30.285196921684022</v>
+      </c>
+      <c r="J52" s="25"/>
+      <c r="K52" s="26" t="e">
+        <f>H52*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L52" s="26" t="e">
+        <f>I52*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M52" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N52" s="28" t="e">
+        <f>(H52*(#REF!/C52))+(I52*(#REF!/C52))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O52" s="28"/>
+      <c r="P52" s="39">
+        <f>0.6128</f>
+        <v>0.61280000000000001</v>
+      </c>
+      <c r="Q52" s="40">
+        <v>282350</v>
+      </c>
+      <c r="R52" s="38">
+        <f t="shared" si="19"/>
+        <v>173024.08000000002</v>
+      </c>
+      <c r="S52" s="38">
+        <f t="shared" si="20"/>
+        <v>109325.91999999998</v>
+      </c>
+      <c r="T52" s="41">
+        <f t="shared" si="21"/>
+        <v>209.60273339972844</v>
+      </c>
+      <c r="U52" s="41">
+        <f t="shared" si="22"/>
+        <v>33.109570158442736</v>
+      </c>
+      <c r="V52" s="66">
+        <f t="shared" si="23"/>
+        <v>85.961502942507948</v>
+      </c>
+      <c r="W52" s="25"/>
+      <c r="X52" s="38">
+        <f t="shared" si="30"/>
+        <v>9</v>
+      </c>
+      <c r="Y52" s="32">
+        <f t="shared" si="24"/>
+        <v>1.2849253055681307</v>
+      </c>
+      <c r="Z52" s="32">
+        <f t="shared" si="29"/>
+        <v>1.2849253055681307</v>
+      </c>
+      <c r="AA52" s="45"/>
+      <c r="AB52" s="46">
+        <f t="shared" si="25"/>
+        <v>85.961502942507948</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="62">
+        <v>1347</v>
+      </c>
+      <c r="C53" s="61">
+        <f t="shared" si="26"/>
+        <v>1654791.1547911547</v>
+      </c>
+      <c r="D53" s="63">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="E53" s="32">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="F53" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" s="25"/>
+      <c r="H53" s="37">
+        <f t="shared" si="27"/>
+        <v>203.88227927363809</v>
+      </c>
+      <c r="I53" s="37">
+        <f t="shared" si="28"/>
+        <v>50.970569818409523</v>
+      </c>
+      <c r="J53" s="25"/>
+      <c r="K53" s="26" t="e">
+        <f>H53*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L53" s="26" t="e">
+        <f>I53*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M53" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N53" s="28" t="e">
+        <f>(H53*(#REF!/C53))+(I53*(#REF!/C53))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O53" s="28"/>
+      <c r="P53" s="39">
+        <f>0.5023</f>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q53" s="40">
+        <v>243989</v>
+      </c>
+      <c r="R53" s="38">
+        <f t="shared" si="19"/>
+        <v>122555.67469999999</v>
+      </c>
+      <c r="S53" s="38">
+        <f t="shared" si="20"/>
+        <v>121433.32530000001</v>
+      </c>
+      <c r="T53" s="41">
+        <f t="shared" si="21"/>
+        <v>249.86930295754541</v>
+      </c>
+      <c r="U53" s="41">
+        <f t="shared" si="22"/>
+        <v>61.895257854852865</v>
+      </c>
+      <c r="V53" s="66">
+        <f t="shared" si="23"/>
+        <v>127.77812147777082</v>
+      </c>
+      <c r="W53" s="25"/>
+      <c r="X53" s="38">
+        <f t="shared" si="30"/>
+        <v>10</v>
+      </c>
+      <c r="Y53" s="32">
+        <f t="shared" si="24"/>
+        <v>1.5697557921102065</v>
+      </c>
+      <c r="Z53" s="32">
+        <f t="shared" si="29"/>
+        <v>1.5697557921102065</v>
+      </c>
+      <c r="AA53" s="45"/>
+      <c r="AB53" s="46">
+        <f t="shared" si="25"/>
+        <v>127.77812147777082</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="62">
+        <v>1290</v>
+      </c>
+      <c r="C54" s="61">
+        <f t="shared" si="26"/>
+        <v>1400651.4657980457</v>
+      </c>
+      <c r="D54" s="63">
+        <v>92.1</v>
+      </c>
+      <c r="E54" s="32">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="37">
+        <f t="shared" si="27"/>
+        <v>230.68252974326862</v>
+      </c>
+      <c r="I54" s="37">
+        <f t="shared" si="28"/>
+        <v>57.670632435817154</v>
+      </c>
+      <c r="J54" s="25"/>
+      <c r="K54" s="26" t="e">
+        <f>H54*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L54" s="26" t="e">
+        <f>I54*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M54" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N54" s="28" t="e">
+        <f>(H54*(#REF!/C54))+(I54*(#REF!/C54))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O54" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="P54" s="39">
+        <f t="shared" ref="P54:P59" si="31">0.5023</f>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q54" s="40">
+        <v>216352</v>
+      </c>
+      <c r="R54" s="38">
+        <f t="shared" si="19"/>
+        <v>108673.6096</v>
+      </c>
+      <c r="S54" s="38">
+        <f t="shared" si="20"/>
+        <v>107678.3904</v>
+      </c>
+      <c r="T54" s="41">
+        <f t="shared" si="21"/>
+        <v>250.69103178860362</v>
+      </c>
+      <c r="U54" s="41">
+        <f t="shared" si="22"/>
+        <v>62.098808740388229</v>
+      </c>
+      <c r="V54" s="66">
+        <f t="shared" si="23"/>
+        <v>144.57450845335003</v>
+      </c>
+      <c r="W54" s="25"/>
+      <c r="X54" s="38">
+        <f t="shared" si="30"/>
+        <v>11</v>
+      </c>
+      <c r="Y54" s="32">
+        <f t="shared" si="24"/>
+        <v>1.5697557921102068</v>
+      </c>
+      <c r="Z54" s="32">
+        <f t="shared" si="29"/>
+        <v>1.5697557921102068</v>
+      </c>
+      <c r="AA54" s="45">
+        <f>AVERAGE(Y54:Y56)</f>
+        <v>1.5677935973700687</v>
+      </c>
+      <c r="AB54" s="46">
+        <f t="shared" si="25"/>
+        <v>144.57450845335003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="62">
+        <v>1136</v>
+      </c>
+      <c r="C55" s="61">
+        <f t="shared" si="26"/>
+        <v>1183333.3333333333</v>
+      </c>
+      <c r="D55" s="63">
+        <v>96</v>
+      </c>
+      <c r="E55" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="F55" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G55" s="25"/>
+      <c r="H55" s="37">
+        <f t="shared" si="27"/>
+        <v>240</v>
+      </c>
+      <c r="I55" s="37">
+        <f t="shared" si="28"/>
+        <v>60</v>
+      </c>
+      <c r="J55" s="25"/>
+      <c r="K55" s="26" t="e">
+        <f>H55*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L55" s="26" t="e">
+        <f>I55*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M55" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N55" s="28" t="e">
+        <f>(H55*(#REF!/C55))+(I55*(#REF!/C55))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O55" s="57"/>
+      <c r="P55" s="39">
+        <f t="shared" si="31"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q55" s="40">
+        <v>189489</v>
+      </c>
+      <c r="R55" s="38">
+        <f t="shared" si="19"/>
+        <v>95180.324699999997</v>
+      </c>
+      <c r="S55" s="38">
+        <f t="shared" si="20"/>
+        <v>94308.675300000003</v>
+      </c>
+      <c r="T55" s="41">
+        <f t="shared" si="21"/>
+        <v>228.43277928000001</v>
+      </c>
+      <c r="U55" s="41">
+        <f t="shared" si="22"/>
+        <v>56.585205180000003</v>
+      </c>
+      <c r="V55" s="66">
+        <f t="shared" si="23"/>
+        <v>150.41399999999999</v>
+      </c>
+      <c r="W55" s="25"/>
+      <c r="X55" s="38">
+        <f t="shared" si="30"/>
+        <v>12</v>
+      </c>
+      <c r="Y55" s="32">
+        <f t="shared" si="24"/>
+        <v>1.5668124999999999</v>
+      </c>
+      <c r="Z55" s="32">
+        <f t="shared" si="29"/>
+        <v>1.5668124999999999</v>
+      </c>
+      <c r="AA55" s="45"/>
+      <c r="AB55" s="46">
+        <f t="shared" si="25"/>
+        <v>150.41399999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="62">
+        <v>960</v>
+      </c>
+      <c r="C56" s="61">
+        <f t="shared" si="26"/>
+        <v>990712.07430340559</v>
+      </c>
+      <c r="D56" s="63">
+        <v>96.9</v>
+      </c>
+      <c r="E56" s="32">
+        <v>0.2</v>
+      </c>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="37">
+        <f t="shared" si="27"/>
+        <v>242.25</v>
+      </c>
+      <c r="I56" s="37">
+        <f t="shared" si="28"/>
+        <v>60.5625</v>
+      </c>
+      <c r="J56" s="25"/>
+      <c r="K56" s="26" t="e">
+        <f>H56*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L56" s="26" t="e">
+        <f>I56*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M56" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N56" s="28" t="e">
+        <f>(H56*(#REF!/C56))+(I56*(#REF!/C56))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O56" s="57"/>
+      <c r="P56" s="39">
+        <f t="shared" si="31"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q56" s="40">
+        <v>163816</v>
+      </c>
+      <c r="R56" s="38">
+        <f t="shared" si="19"/>
+        <v>82284.776799999992</v>
+      </c>
+      <c r="S56" s="38">
+        <f t="shared" si="20"/>
+        <v>81531.223200000008</v>
+      </c>
+      <c r="T56" s="41">
+        <f t="shared" si="21"/>
+        <v>199.33487179799997</v>
+      </c>
+      <c r="U56" s="41">
+        <f t="shared" si="22"/>
+        <v>49.377347050500006</v>
+      </c>
+      <c r="V56" s="66">
+        <f t="shared" si="23"/>
+        <v>151.82413124999997</v>
+      </c>
+      <c r="W56" s="25"/>
+      <c r="X56" s="38">
+        <f t="shared" si="30"/>
+        <v>13</v>
+      </c>
+      <c r="Y56" s="32">
+        <f t="shared" si="24"/>
+        <v>1.5668124999999995</v>
+      </c>
+      <c r="Z56" s="32">
+        <f t="shared" si="29"/>
+        <v>1.5668124999999995</v>
+      </c>
+      <c r="AA56" s="45"/>
+      <c r="AB56" s="46">
+        <f t="shared" si="25"/>
+        <v>151.82413124999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" s="62">
+        <v>742</v>
+      </c>
+      <c r="C57" s="61">
+        <f t="shared" si="26"/>
+        <v>785185.18518518517</v>
+      </c>
+      <c r="D57" s="63">
+        <v>94.5</v>
+      </c>
+      <c r="E57" s="32">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="F57" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G57" s="25"/>
+      <c r="H57" s="37">
+        <f t="shared" si="27"/>
+        <v>326.14322691975838</v>
+      </c>
+      <c r="I57" s="37">
+        <f t="shared" si="28"/>
+        <v>81.535806729939594</v>
+      </c>
+      <c r="J57" s="25"/>
+      <c r="K57" s="26" t="e">
+        <f>H57*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L57" s="26" t="e">
+        <f>I57*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M57" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N57" s="28" t="e">
+        <f>(H57*(#REF!/C57))+(I57*(#REF!/C57))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O57" s="57"/>
+      <c r="P57" s="39">
+        <f t="shared" si="31"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q57" s="40">
+        <v>134732</v>
+      </c>
+      <c r="R57" s="38">
+        <f t="shared" si="19"/>
+        <v>67675.883600000001</v>
+      </c>
+      <c r="S57" s="38">
+        <f t="shared" si="20"/>
+        <v>67056.116399999999</v>
+      </c>
+      <c r="T57" s="41">
+        <f t="shared" si="21"/>
+        <v>220.72031061949954</v>
+      </c>
+      <c r="U57" s="41">
+        <f t="shared" si="22"/>
+        <v>54.674745468507325</v>
+      </c>
+      <c r="V57" s="66">
+        <f t="shared" si="23"/>
+        <v>204.40211389128555</v>
+      </c>
+      <c r="W57" s="25"/>
+      <c r="X57" s="38">
+        <f t="shared" si="30"/>
+        <v>14</v>
+      </c>
+      <c r="Y57" s="32">
+        <f t="shared" si="24"/>
+        <v>2.1629853321829158</v>
+      </c>
+      <c r="Z57" s="32">
+        <f>Z56</f>
+        <v>1.5668124999999995</v>
+      </c>
+      <c r="AA57" s="45"/>
+      <c r="AB57" s="46">
+        <f t="shared" si="25"/>
+        <v>148.06378124999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="62">
+        <v>519</v>
+      </c>
+      <c r="C58" s="61">
+        <f t="shared" si="26"/>
+        <v>536157.02479338844</v>
+      </c>
+      <c r="D58" s="63">
+        <v>96.8</v>
+      </c>
+      <c r="E58" s="32">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="37">
+        <f t="shared" si="27"/>
+        <v>334.08110440034511</v>
+      </c>
+      <c r="I58" s="37">
+        <f t="shared" si="28"/>
+        <v>83.520276100086278</v>
+      </c>
+      <c r="J58" s="25"/>
+      <c r="K58" s="26" t="e">
+        <f>H58*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L58" s="26" t="e">
+        <f>I58*#REF!/100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M58" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="N58" s="28" t="e">
+        <f>(H58*(#REF!/C58))+(I58*(#REF!/C58))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="O58" s="57"/>
+      <c r="P58" s="39">
+        <f t="shared" si="31"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q58" s="40">
+        <v>93602</v>
+      </c>
+      <c r="R58" s="38">
+        <f t="shared" si="19"/>
+        <v>47016.284599999999</v>
+      </c>
+      <c r="S58" s="38">
+        <f t="shared" si="20"/>
+        <v>46585.715400000001</v>
+      </c>
+      <c r="T58" s="41">
+        <f t="shared" si="21"/>
+        <v>157.07252283968938</v>
+      </c>
+      <c r="U58" s="41">
+        <f t="shared" si="22"/>
+        <v>38.908518125280409</v>
+      </c>
+      <c r="V58" s="66">
+        <f t="shared" si="23"/>
+        <v>209.37698015530628</v>
+      </c>
+      <c r="W58" s="25"/>
+      <c r="X58" s="38">
+        <f t="shared" si="30"/>
+        <v>15</v>
+      </c>
+      <c r="Y58" s="32">
+        <f t="shared" si="24"/>
+        <v>2.1629853321829162</v>
+      </c>
+      <c r="Z58" s="32">
+        <f t="shared" ref="Z58" si="32">Z57</f>
+        <v>1.5668124999999995</v>
+      </c>
+      <c r="AA58" s="45"/>
+      <c r="AB58" s="46">
+        <f t="shared" si="25"/>
+        <v>151.66744999999995</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="32">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="37" t="e">
+        <f t="shared" ref="H47:H59" si="33">I$1*I59</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I59" s="37" t="e">
+        <f t="shared" ref="I47:I59" si="34">D59/(I$1*E59+(1-E59))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J59" s="25"/>
+      <c r="K59" s="26" t="e">
+        <f>H59*#REF!/100000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L59" s="26" t="e">
+        <f>I59*#REF!/100000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M59" s="26" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N59" s="28" t="e">
+        <f>(H59*(#REF!/C59))+(I59*(#REF!/C59))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O59" s="57"/>
+      <c r="P59" s="39">
+        <f t="shared" si="31"/>
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="Q59" s="40">
+        <v>58431</v>
+      </c>
+      <c r="R59" s="38">
+        <f t="shared" si="19"/>
+        <v>29349.891299999999</v>
+      </c>
+      <c r="S59" s="38">
+        <f t="shared" si="20"/>
+        <v>29081.108700000001</v>
+      </c>
+      <c r="T59" s="41" t="e">
+        <f t="shared" si="21"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U59" s="41" t="e">
+        <f t="shared" si="22"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V59" s="41" t="e">
+        <f t="shared" si="23"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W59" s="25"/>
+      <c r="X59" s="38">
+        <f t="shared" si="30"/>
+        <v>16</v>
+      </c>
+      <c r="Y59" s="32" t="e">
+        <f t="shared" si="24"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z59" s="32"/>
+      <c r="AA59" s="32"/>
+      <c r="AB59" s="46"/>
+    </row>
+    <row r="60" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="25"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="25"/>
+      <c r="K60" s="25"/>
+      <c r="L60" s="25"/>
+      <c r="M60" s="25"/>
+      <c r="N60" s="25"/>
+      <c r="O60" s="25"/>
+      <c r="P60" s="25"/>
+      <c r="Q60" s="25"/>
+      <c r="R60" s="25"/>
+      <c r="S60" s="25"/>
+      <c r="T60" s="25"/>
+      <c r="U60" s="25"/>
+      <c r="V60" s="25"/>
+      <c r="W60" s="25"/>
+      <c r="X60" s="25"/>
+      <c r="Y60" s="25"/>
+      <c r="Z60" s="25"/>
+      <c r="AA60" s="26"/>
+      <c r="AB60" s="50"/>
+    </row>
+    <row r="61" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" s="27">
+        <f>SUM(B47:B58)</f>
+        <v>9886</v>
+      </c>
+      <c r="C61" s="27">
+        <f>SUM(C47:C58)</f>
+        <v>20986475.734300051</v>
+      </c>
+      <c r="D61" s="28">
+        <f>B61/C61*100000</f>
+        <v>47.106527676023454</v>
+      </c>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="29" t="e">
+        <f>K61/#REF!*100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I61" s="29" t="e">
+        <f>L61/#REF!*100000</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J61" s="25"/>
+      <c r="K61" s="26" t="e">
+        <f t="shared" ref="K61:L61" si="35">SUM(K47:K59)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L61" s="26" t="e">
+        <f t="shared" si="35"/>
+        <v>#REF!</v>
+      </c>
+      <c r="M61" s="26"/>
+      <c r="N61" s="25"/>
+      <c r="O61" s="30"/>
+      <c r="P61" s="25"/>
+      <c r="Q61" s="27">
+        <f t="shared" ref="Q61:U61" si="36">SUM(Q47:Q59)</f>
+        <v>3789911</v>
+      </c>
+      <c r="R61" s="26">
+        <f t="shared" si="36"/>
+        <v>1750735.6040000003</v>
+      </c>
+      <c r="S61" s="26">
+        <f t="shared" si="36"/>
+        <v>2039175.3959999997</v>
+      </c>
+      <c r="T61" s="29" t="e">
+        <f t="shared" si="36"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U61" s="29" t="e">
+        <f t="shared" si="36"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V61" s="29" t="e">
+        <f>(T61+U61)/Q61*100000</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W61" s="25"/>
+      <c r="X61" s="25"/>
+      <c r="Y61" s="27"/>
+      <c r="Z61" s="27"/>
+      <c r="AA61" s="26"/>
+      <c r="AB61" s="18"/>
+    </row>
+    <row r="62" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4948,7 +7714,12 @@
     <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="R45:S45"/>
+    <mergeCell ref="T45:V45"/>
+    <mergeCell ref="O54:O59"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="H2:I2"/>
@@ -5014,9 +7785,9 @@
       <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -5029,34 +7800,34 @@
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
+      <c r="A20" s="58"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Fix Excel plot title
</commit_message>
<xml_diff>
--- a/Config/Reweighted_GlobocanCC_rates.xlsx
+++ b/Config/Reweighted_GlobocanCC_rates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\HHCoM\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D721F470-CBAD-480F-B754-A11E9558C10A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2169E827-762D-40CF-806E-C290C198D9AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="387" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,25 +523,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -560,6 +541,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,7 +1307,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Globocan 2018 for KZN</a:t>
+              <a:t> Globocan 2020 for KZN</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3350,8 +3350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE959"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB47" sqref="AB47:AB58"/>
+    <sheetView tabSelected="1" topLeftCell="I43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V91" sqref="V91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3419,20 +3419,20 @@
     </row>
     <row r="2" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="52" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="56"/>
+      <c r="I2" s="65"/>
       <c r="J2" s="25"/>
       <c r="K2" s="24" t="s">
         <v>1</v>
@@ -3447,22 +3447,22 @@
       <c r="Q2" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="R2" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="56"/>
-      <c r="T2" s="54" t="s">
+      <c r="S2" s="65"/>
+      <c r="T2" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
       <c r="W2" s="25"/>
       <c r="X2" s="47"/>
       <c r="Y2" s="25"/>
       <c r="Z2" s="25"/>
       <c r="AA2" s="26"/>
     </row>
-    <row r="3" spans="1:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>2</v>
       </c>
@@ -3629,7 +3629,7 @@
         <f>AVERAGE(Y4:Y6)</f>
         <v>1.2195984455181634</v>
       </c>
-      <c r="AB4" s="67">
+      <c r="AB4" s="60">
         <f t="shared" ref="AB4:AB15" si="9">D4*Z4</f>
         <v>4.2506211395658813</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>1.3341772151898736</v>
       </c>
       <c r="AA5" s="45"/>
-      <c r="AB5" s="67">
+      <c r="AB5" s="60">
         <f t="shared" si="9"/>
         <v>26.308096902593544</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>1.2366826923076921</v>
       </c>
       <c r="AA6" s="45"/>
-      <c r="AB6" s="67">
+      <c r="AB6" s="60">
         <f t="shared" si="9"/>
         <v>44.29228102011205</v>
       </c>
@@ -3916,7 +3916,7 @@
         <f>AVERAGE(Y7:Y10)</f>
         <v>1.4018326814868265</v>
       </c>
-      <c r="AB7" s="67">
+      <c r="AB7" s="60">
         <f t="shared" si="9"/>
         <v>74.756761777182135</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>1.3619284744228155</v>
       </c>
       <c r="AA8" s="45"/>
-      <c r="AB8" s="67">
+      <c r="AB8" s="60">
         <f t="shared" si="9"/>
         <v>96.943788621935781</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>1.2849253055681302</v>
       </c>
       <c r="AA9" s="45"/>
-      <c r="AB9" s="67">
+      <c r="AB9" s="60">
         <f t="shared" si="9"/>
         <v>109.33496137495494</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>1.5697557921102063</v>
       </c>
       <c r="AA10" s="45"/>
-      <c r="AB10" s="67">
+      <c r="AB10" s="60">
         <f t="shared" si="9"/>
         <v>149.82317295754092</v>
       </c>
@@ -4254,7 +4254,7 @@
         <f>(H11*(#REF!/C11))+(I11*(#REF!/C11))</f>
         <v>#REF!</v>
       </c>
-      <c r="O11" s="57" t="s">
+      <c r="O11" s="66" t="s">
         <v>37</v>
       </c>
       <c r="P11" s="39">
@@ -4301,7 +4301,7 @@
         <f>AVERAGE(Y11:Y13)</f>
         <v>1.5677935973700687</v>
       </c>
-      <c r="AB11" s="67">
+      <c r="AB11" s="60">
         <f t="shared" si="9"/>
         <v>150.85278467194186</v>
       </c>
@@ -4355,7 +4355,7 @@
         <f>(H12*(#REF!/C12))+(I12*(#REF!/C12))</f>
         <v>#REF!</v>
       </c>
-      <c r="O12" s="57"/>
+      <c r="O12" s="66"/>
       <c r="P12" s="39">
         <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
@@ -4397,7 +4397,7 @@
         <v>1.5668124999999999</v>
       </c>
       <c r="AA12" s="45"/>
-      <c r="AB12" s="67">
+      <c r="AB12" s="60">
         <f t="shared" si="9"/>
         <v>148.61463801411369</v>
       </c>
@@ -4449,7 +4449,7 @@
         <f>(H13*(#REF!/C13))+(I13*(#REF!/C13))</f>
         <v>#REF!</v>
       </c>
-      <c r="O13" s="57"/>
+      <c r="O13" s="66"/>
       <c r="P13" s="39">
         <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
@@ -4491,7 +4491,7 @@
         <v>1.5668124999999997</v>
       </c>
       <c r="AA13" s="45"/>
-      <c r="AB13" s="67">
+      <c r="AB13" s="60">
         <f t="shared" si="9"/>
         <v>152.74467502139476</v>
       </c>
@@ -4545,7 +4545,7 @@
         <f>(H14*(#REF!/C14))+(I14*(#REF!/C14))</f>
         <v>#REF!</v>
       </c>
-      <c r="O14" s="57"/>
+      <c r="O14" s="66"/>
       <c r="P14" s="39">
         <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
@@ -4587,7 +4587,7 @@
         <v>1.5668124999999997</v>
       </c>
       <c r="AA14" s="45"/>
-      <c r="AB14" s="67">
+      <c r="AB14" s="60">
         <f t="shared" si="9"/>
         <v>159.7964462557934</v>
       </c>
@@ -4639,7 +4639,7 @@
         <f>(H15*(#REF!/C15))+(I15*(#REF!/C15))</f>
         <v>#REF!</v>
       </c>
-      <c r="O15" s="57"/>
+      <c r="O15" s="66"/>
       <c r="P15" s="39">
         <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
@@ -4681,7 +4681,7 @@
         <v>1.5668124999999997</v>
       </c>
       <c r="AA15" s="45"/>
-      <c r="AB15" s="67">
+      <c r="AB15" s="60">
         <f t="shared" si="9"/>
         <v>173.01551552043256</v>
       </c>
@@ -4732,7 +4732,7 @@
         <f>(H16*(#REF!/C16))+(I16*(#REF!/C16))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O16" s="57"/>
+      <c r="O16" s="66"/>
       <c r="P16" s="39">
         <f t="shared" si="13"/>
         <v>0.50229999999999997</v>
@@ -5398,20 +5398,20 @@
     </row>
     <row r="45" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
-      <c r="B45" s="60" t="s">
+      <c r="B45" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="52" t="s">
         <v>25</v>
       </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="55" t="s">
+      <c r="H45" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="I45" s="56"/>
+      <c r="I45" s="65"/>
       <c r="J45" s="25"/>
       <c r="K45" s="24" t="s">
         <v>1</v>
@@ -5426,15 +5426,15 @@
       <c r="Q45" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="R45" s="55" t="s">
+      <c r="R45" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="S45" s="56"/>
-      <c r="T45" s="54" t="s">
+      <c r="S45" s="65"/>
+      <c r="T45" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="U45" s="54"/>
-      <c r="V45" s="54"/>
+      <c r="U45" s="63"/>
+      <c r="V45" s="63"/>
       <c r="W45" s="25"/>
       <c r="X45" s="47"/>
       <c r="Y45" s="25"/>
@@ -5442,7 +5442,7 @@
       <c r="AA45" s="26"/>
       <c r="AB45" s="50"/>
     </row>
-    <row r="46" spans="1:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
         <v>2</v>
       </c>
@@ -5505,7 +5505,7 @@
       <c r="X46" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="Y46" s="68" t="s">
+      <c r="Y46" s="61" t="s">
         <v>54</v>
       </c>
       <c r="Z46" s="42" t="s">
@@ -5522,14 +5522,14 @@
       <c r="A47" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B47" s="62">
+      <c r="B47" s="55">
         <v>14</v>
       </c>
-      <c r="C47" s="61">
+      <c r="C47" s="54">
         <f>B47/(D47/100000)</f>
         <v>2456140.3508771933</v>
       </c>
-      <c r="D47" s="63">
+      <c r="D47" s="56">
         <v>0.56999999999999995</v>
       </c>
       <c r="E47" s="32">
@@ -5586,7 +5586,7 @@
         <f t="shared" ref="U47:U59" si="22">I47*S47/100000</f>
         <v>2.3629924963891247</v>
       </c>
-      <c r="V47" s="66">
+      <c r="V47" s="59">
         <f t="shared" ref="V47:V59" si="23">(T47+U47)/Q47*100000</f>
         <v>0.6201231945624468</v>
       </c>
@@ -5615,14 +5615,14 @@
       <c r="A48" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="62">
+      <c r="B48" s="55">
         <v>114</v>
       </c>
-      <c r="C48" s="61">
+      <c r="C48" s="54">
         <f t="shared" ref="C48:C58" si="26">B48/(D48/100000)</f>
         <v>2425531.9148936169</v>
       </c>
-      <c r="D48" s="63">
+      <c r="D48" s="56">
         <v>4.7</v>
       </c>
       <c r="E48" s="32">
@@ -5679,7 +5679,7 @@
         <f t="shared" si="22"/>
         <v>11.33382113724184</v>
       </c>
-      <c r="V48" s="66">
+      <c r="V48" s="59">
         <f t="shared" si="23"/>
         <v>6.2706329113924051</v>
       </c>
@@ -5706,14 +5706,14 @@
       <c r="A49" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="62">
+      <c r="B49" s="55">
         <v>459</v>
       </c>
-      <c r="C49" s="61">
+      <c r="C49" s="54">
         <f t="shared" si="26"/>
         <v>2593220.338983051</v>
       </c>
-      <c r="D49" s="63">
+      <c r="D49" s="56">
         <v>17.7</v>
       </c>
       <c r="E49" s="32">
@@ -5772,7 +5772,7 @@
         <f t="shared" si="22"/>
         <v>21.4563390839423</v>
       </c>
-      <c r="V49" s="66">
+      <c r="V49" s="59">
         <f t="shared" si="23"/>
         <v>21.889283653846149</v>
       </c>
@@ -5799,14 +5799,14 @@
       <c r="A50" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B50" s="62">
+      <c r="B50" s="55">
         <v>851</v>
       </c>
-      <c r="C50" s="61">
+      <c r="C50" s="54">
         <f t="shared" si="26"/>
         <v>2667711.5987460813</v>
       </c>
-      <c r="D50" s="63">
+      <c r="D50" s="56">
         <v>31.9</v>
       </c>
       <c r="E50" s="32">
@@ -5863,7 +5863,7 @@
         <f t="shared" si="22"/>
         <v>25.298590458413457</v>
       </c>
-      <c r="V50" s="66">
+      <c r="V50" s="59">
         <f t="shared" si="23"/>
         <v>44.364004807692304</v>
       </c>
@@ -5893,14 +5893,14 @@
       <c r="A51" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="62">
+      <c r="B51" s="55">
         <v>1171</v>
       </c>
-      <c r="C51" s="61">
+      <c r="C51" s="54">
         <f t="shared" si="26"/>
         <v>2375253.5496957405</v>
       </c>
-      <c r="D51" s="63">
+      <c r="D51" s="56">
         <v>49.3</v>
       </c>
       <c r="E51" s="32">
@@ -5959,7 +5959,7 @@
         <f t="shared" si="22"/>
         <v>25.705685404934357</v>
       </c>
-      <c r="V51" s="66">
+      <c r="V51" s="59">
         <f t="shared" si="23"/>
         <v>67.143073789044792</v>
       </c>
@@ -5986,14 +5986,14 @@
       <c r="A52" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="62">
+      <c r="B52" s="55">
         <v>1283</v>
       </c>
-      <c r="C52" s="61">
+      <c r="C52" s="54">
         <f t="shared" si="26"/>
         <v>1917787.7428998502</v>
       </c>
-      <c r="D52" s="63">
+      <c r="D52" s="56">
         <v>66.900000000000006</v>
       </c>
       <c r="E52" s="32">
@@ -6050,7 +6050,7 @@
         <f t="shared" si="22"/>
         <v>33.109570158442736</v>
       </c>
-      <c r="V52" s="66">
+      <c r="V52" s="59">
         <f t="shared" si="23"/>
         <v>85.961502942507948</v>
       </c>
@@ -6077,14 +6077,14 @@
       <c r="A53" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="62">
+      <c r="B53" s="55">
         <v>1347</v>
       </c>
-      <c r="C53" s="61">
+      <c r="C53" s="54">
         <f t="shared" si="26"/>
         <v>1654791.1547911547</v>
       </c>
-      <c r="D53" s="63">
+      <c r="D53" s="56">
         <v>81.400000000000006</v>
       </c>
       <c r="E53" s="32">
@@ -6143,7 +6143,7 @@
         <f t="shared" si="22"/>
         <v>61.895257854852865</v>
       </c>
-      <c r="V53" s="66">
+      <c r="V53" s="59">
         <f t="shared" si="23"/>
         <v>127.77812147777082</v>
       </c>
@@ -6170,14 +6170,14 @@
       <c r="A54" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="62">
+      <c r="B54" s="55">
         <v>1290</v>
       </c>
-      <c r="C54" s="61">
+      <c r="C54" s="54">
         <f t="shared" si="26"/>
         <v>1400651.4657980457</v>
       </c>
-      <c r="D54" s="63">
+      <c r="D54" s="56">
         <v>92.1</v>
       </c>
       <c r="E54" s="32">
@@ -6210,7 +6210,7 @@
         <f>(H54*(#REF!/C54))+(I54*(#REF!/C54))</f>
         <v>#REF!</v>
       </c>
-      <c r="O54" s="57" t="s">
+      <c r="O54" s="66" t="s">
         <v>37</v>
       </c>
       <c r="P54" s="39">
@@ -6236,7 +6236,7 @@
         <f t="shared" si="22"/>
         <v>62.098808740388229</v>
       </c>
-      <c r="V54" s="66">
+      <c r="V54" s="59">
         <f t="shared" si="23"/>
         <v>144.57450845335003</v>
       </c>
@@ -6266,14 +6266,14 @@
       <c r="A55" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="62">
+      <c r="B55" s="55">
         <v>1136</v>
       </c>
-      <c r="C55" s="61">
+      <c r="C55" s="54">
         <f t="shared" si="26"/>
         <v>1183333.3333333333</v>
       </c>
-      <c r="D55" s="63">
+      <c r="D55" s="56">
         <v>96</v>
       </c>
       <c r="E55" s="32">
@@ -6308,7 +6308,7 @@
         <f>(H55*(#REF!/C55))+(I55*(#REF!/C55))</f>
         <v>#REF!</v>
       </c>
-      <c r="O55" s="57"/>
+      <c r="O55" s="66"/>
       <c r="P55" s="39">
         <f t="shared" si="31"/>
         <v>0.50229999999999997</v>
@@ -6332,7 +6332,7 @@
         <f t="shared" si="22"/>
         <v>56.585205180000003</v>
       </c>
-      <c r="V55" s="66">
+      <c r="V55" s="59">
         <f t="shared" si="23"/>
         <v>150.41399999999999</v>
       </c>
@@ -6359,14 +6359,14 @@
       <c r="A56" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="62">
+      <c r="B56" s="55">
         <v>960</v>
       </c>
-      <c r="C56" s="61">
+      <c r="C56" s="54">
         <f t="shared" si="26"/>
         <v>990712.07430340559</v>
       </c>
-      <c r="D56" s="63">
+      <c r="D56" s="56">
         <v>96.9</v>
       </c>
       <c r="E56" s="32">
@@ -6399,7 +6399,7 @@
         <f>(H56*(#REF!/C56))+(I56*(#REF!/C56))</f>
         <v>#REF!</v>
       </c>
-      <c r="O56" s="57"/>
+      <c r="O56" s="66"/>
       <c r="P56" s="39">
         <f t="shared" si="31"/>
         <v>0.50229999999999997</v>
@@ -6423,7 +6423,7 @@
         <f t="shared" si="22"/>
         <v>49.377347050500006</v>
       </c>
-      <c r="V56" s="66">
+      <c r="V56" s="59">
         <f t="shared" si="23"/>
         <v>151.82413124999997</v>
       </c>
@@ -6450,14 +6450,14 @@
       <c r="A57" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B57" s="62">
+      <c r="B57" s="55">
         <v>742</v>
       </c>
-      <c r="C57" s="61">
+      <c r="C57" s="54">
         <f t="shared" si="26"/>
         <v>785185.18518518517</v>
       </c>
-      <c r="D57" s="63">
+      <c r="D57" s="56">
         <v>94.5</v>
       </c>
       <c r="E57" s="32">
@@ -6492,7 +6492,7 @@
         <f>(H57*(#REF!/C57))+(I57*(#REF!/C57))</f>
         <v>#REF!</v>
       </c>
-      <c r="O57" s="57"/>
+      <c r="O57" s="66"/>
       <c r="P57" s="39">
         <f t="shared" si="31"/>
         <v>0.50229999999999997</v>
@@ -6516,7 +6516,7 @@
         <f t="shared" si="22"/>
         <v>54.674745468507325</v>
       </c>
-      <c r="V57" s="66">
+      <c r="V57" s="59">
         <f t="shared" si="23"/>
         <v>204.40211389128555</v>
       </c>
@@ -6543,14 +6543,14 @@
       <c r="A58" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="62">
+      <c r="B58" s="55">
         <v>519</v>
       </c>
-      <c r="C58" s="61">
+      <c r="C58" s="54">
         <f t="shared" si="26"/>
         <v>536157.02479338844</v>
       </c>
-      <c r="D58" s="63">
+      <c r="D58" s="56">
         <v>96.8</v>
       </c>
       <c r="E58" s="32">
@@ -6583,7 +6583,7 @@
         <f>(H58*(#REF!/C58))+(I58*(#REF!/C58))</f>
         <v>#REF!</v>
       </c>
-      <c r="O58" s="57"/>
+      <c r="O58" s="66"/>
       <c r="P58" s="39">
         <f t="shared" si="31"/>
         <v>0.50229999999999997</v>
@@ -6607,7 +6607,7 @@
         <f t="shared" si="22"/>
         <v>38.908518125280409</v>
       </c>
-      <c r="V58" s="66">
+      <c r="V58" s="59">
         <f t="shared" si="23"/>
         <v>209.37698015530628</v>
       </c>
@@ -6634,13 +6634,13 @@
       <c r="A59" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="64" t="s">
+      <c r="B59" s="57" t="s">
         <v>19</v>
       </c>
       <c r="C59" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D59" s="65" t="s">
+      <c r="D59" s="58" t="s">
         <v>19</v>
       </c>
       <c r="E59" s="32">
@@ -6649,11 +6649,11 @@
       <c r="F59" s="25"/>
       <c r="G59" s="25"/>
       <c r="H59" s="37" t="e">
-        <f t="shared" ref="H47:H59" si="33">I$1*I59</f>
+        <f t="shared" ref="H59" si="33">I$1*I59</f>
         <v>#VALUE!</v>
       </c>
       <c r="I59" s="37" t="e">
-        <f t="shared" ref="I47:I59" si="34">D59/(I$1*E59+(1-E59))</f>
+        <f t="shared" ref="I59" si="34">D59/(I$1*E59+(1-E59))</f>
         <v>#VALUE!</v>
       </c>
       <c r="J59" s="25"/>
@@ -6673,7 +6673,7 @@
         <f>(H59*(#REF!/C59))+(I59*(#REF!/C59))</f>
         <v>#VALUE!</v>
       </c>
-      <c r="O59" s="57"/>
+      <c r="O59" s="66"/>
       <c r="P59" s="39">
         <f t="shared" si="31"/>
         <v>0.50229999999999997</v>
@@ -7715,16 +7715,16 @@
     <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="O11:O16"/>
+    <mergeCell ref="R2:S2"/>
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="R45:S45"/>
     <mergeCell ref="T45:V45"/>
     <mergeCell ref="O54:O59"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="O11:O16"/>
-    <mergeCell ref="R2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7785,9 +7785,9 @@
       <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="58"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -7800,34 +7800,34 @@
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="58"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="58"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>